<commit_message>
Updated DC with an example for gAUC LGD
</commit_message>
<xml_diff>
--- a/IRB models/Data Model.xlsx
+++ b/IRB models/Data Model.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bebxadvsven\Documents\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bebxadvboey\Documents\Python\GitHub\ML4Credit\IRB models\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1F508E75-2F51-489E-9856-8A8D22AC95EC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" state="hidden" r:id="rId1"/>
@@ -20,10 +21,11 @@
     <sheet name="DataModel" sheetId="17" r:id="rId6"/>
     <sheet name="New structure" sheetId="18" r:id="rId7"/>
     <sheet name="Data Catalogue" sheetId="19" r:id="rId8"/>
-    <sheet name="Data Fact Sheet" sheetId="12" state="hidden" r:id="rId9"/>
+    <sheet name="DataCatalogue" sheetId="20" r:id="rId9"/>
+    <sheet name="Data Fact Sheet" sheetId="12" state="hidden" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">browseNotes!$A$1:$B$89</definedName>
@@ -31,7 +33,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
-  <calcPr calcId="171027" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="179017" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -41,12 +43,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sander Vandevenne</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -70,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -101,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -125,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
         <r>
           <rPr>
@@ -150,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
       <text>
         <r>
           <rPr>
@@ -180,12 +182,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Brent Oeyen</author>
   </authors>
   <commentList>
-    <comment ref="E9" authorId="0" shapeId="0">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -214,12 +216,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sander Vandevenne</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
@@ -243,7 +245,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000002000000}">
       <text>
         <r>
           <rPr>
@@ -267,7 +269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000003000000}">
       <text>
         <r>
           <rPr>
@@ -292,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000004000000}">
       <text>
         <r>
           <rPr>
@@ -316,7 +318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000005000000}">
       <text>
         <r>
           <rPr>
@@ -340,7 +342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000006000000}">
       <text>
         <r>
           <rPr>
@@ -364,7 +366,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000007000000}">
       <text>
         <r>
           <rPr>
@@ -388,7 +390,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000008000000}">
       <text>
         <r>
           <rPr>
@@ -412,7 +414,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H23" authorId="0" shapeId="0">
+    <comment ref="H23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000009000000}">
       <text>
         <r>
           <rPr>
@@ -442,7 +444,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="814">
   <si>
     <t>LoanStatNew</t>
   </si>
@@ -2801,11 +2803,142 @@
   <si>
     <t>Scaled interest rate on the facility</t>
   </si>
+  <si>
+    <t>Data layer</t>
+  </si>
+  <si>
+    <t>Section 2.6.1(b)</t>
+  </si>
+  <si>
+    <t>Section 2.6.1(a)</t>
+  </si>
+  <si>
+    <t>bin_LGD</t>
+  </si>
+  <si>
+    <t>bin_LGD_realised</t>
+  </si>
+  <si>
+    <t>Section 2.3(c ) with default =1 and performing = 0</t>
+  </si>
+  <si>
+    <t>dev_LGD_transition_matrix_freq</t>
+  </si>
+  <si>
+    <t>mon_LGD_transition_matrix_freq</t>
+  </si>
+  <si>
+    <t>LGD_gAUC_init</t>
+  </si>
+  <si>
+    <t>LGD_gAUC_curr</t>
+  </si>
+  <si>
+    <t>LGD_S</t>
+  </si>
+  <si>
+    <t>LGD_p_val</t>
+  </si>
+  <si>
+    <t>Code ref</t>
+  </si>
+  <si>
+    <t>Section 3.2: Facility pools used by the institution or 12 percentile intervals based on LGD ordered from low to high</t>
+  </si>
+  <si>
+    <t>Section 3.2: Facility pools used by the institution or 12 percentile intervals based on realised LGD  ordered from low to high</t>
+  </si>
+  <si>
+    <t>Section 3.2: referred to as a for the development period</t>
+  </si>
+  <si>
+    <t>Section 3.2: reference a divided by c for the development period</t>
+  </si>
+  <si>
+    <t>Section 3.2: reference a divided by c for the validation period</t>
+  </si>
+  <si>
+    <t>Section 3.2: referred to as a for the validation period</t>
+  </si>
+  <si>
+    <t>Section 3.2: AUC calculated for the development period</t>
+  </si>
+  <si>
+    <t>Section 3.2: AUC calculated for the validation period</t>
+  </si>
+  <si>
+    <t>Section 3.2: P-value test statistic of AUC for the validation period</t>
+  </si>
+  <si>
+    <t>Type variable</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Regulatory ref</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_LGD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 3.0      cell: D7</t>
+  </si>
+  <si>
+    <t>export</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_LGD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 3.0      cell: E7</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_LGD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 3.0      cell: F7</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_LGD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 3.0      cell: G7</t>
+  </si>
+  <si>
+    <t>Section 3.2: Test statistic of the AUC calculated for the validation period</t>
+  </si>
+  <si>
+    <t>LGD_s</t>
+  </si>
+  <si>
+    <t>Section 3.2: Variance</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_LGD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 3.0      cell: H7</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Script calc</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>LGD_tests</t>
+  </si>
+  <si>
+    <t>matrix</t>
+  </si>
+  <si>
+    <t>matrix_obs</t>
+  </si>
+  <si>
+    <t>matrix_prob</t>
+  </si>
+  <si>
+    <t>LGD_toExcel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3726,7 +3859,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3885,6 +4018,13 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="37" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3933,13 +4073,7 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="88">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4699,19 +4833,7 @@
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
-                        <m:t>+</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="nl-BE" sz="1100" b="0" i="1">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1"/>
-                          </a:solidFill>
-                          <a:effectLst/>
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:rPr>
-                        <m:t>1</m:t>
+                        <m:t>+1</m:t>
                       </m:r>
                     </m:sub>
                     <m:sup>
@@ -6458,7 +6580,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -7119,7 +7241,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B57">
+  <autoFilter ref="A1:B57" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="A2:B61">
       <sortCondition ref="A1:A61"/>
     </sortState>
@@ -7137,8 +7259,301 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet7"/>
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="31" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="91" t="s">
+        <v>562</v>
+      </c>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="93"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="94"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="96"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="87" t="s">
+        <v>563</v>
+      </c>
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="89"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>564</v>
+      </c>
+      <c r="B5" s="97" t="s">
+        <v>565</v>
+      </c>
+      <c r="C5" s="98"/>
+      <c r="D5" s="99"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
+        <v>566</v>
+      </c>
+      <c r="B6" s="97" t="s">
+        <v>567</v>
+      </c>
+      <c r="C6" s="98"/>
+      <c r="D6" s="99"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="33" t="s">
+        <v>568</v>
+      </c>
+      <c r="B7" s="100" t="s">
+        <v>569</v>
+      </c>
+      <c r="C7" s="101"/>
+      <c r="D7" s="102"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="34" t="s">
+        <v>570</v>
+      </c>
+      <c r="B8" s="100" t="s">
+        <v>571</v>
+      </c>
+      <c r="C8" s="101"/>
+      <c r="D8" s="102"/>
+    </row>
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="87" t="s">
+        <v>572</v>
+      </c>
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="89"/>
+    </row>
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>573</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>574</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>575</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
+        <v>576</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>577</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>578</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="32" t="s">
+        <v>580</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>581</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>582</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="33" t="s">
+        <v>584</v>
+      </c>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+    </row>
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="33"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+    </row>
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="90" t="s">
+        <v>585</v>
+      </c>
+      <c r="B17" s="90"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+    </row>
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
+          <x14:formula1>
+            <xm:f>'Z:\FSO Advisory All\2. FSO Advisory _ Solutions\3. Risk\2. Data Quality\1. Conceptual\[DataQuality_Testing_Conceptual.xlsb]Lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>C12:D13</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -7157,7 +7572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B109"/>
   <sheetViews>
@@ -8035,7 +8450,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B89">
+  <autoFilter ref="A1:B89" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <sortState ref="A2:B93">
       <sortCondition ref="A1:A93"/>
     </sortState>
@@ -8054,7 +8469,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -8152,7 +8567,7 @@
       <c r="B12" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B10"/>
+  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -8165,7 +8580,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5">
     <tabColor theme="4"/>
   </sheetPr>
@@ -8641,12 +9056,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K247"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
@@ -12403,7 +12818,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
         <mc:Choice Requires="x12ac">
           <x12ac:list>"{""a"",""b""}"</x12ac:list>
@@ -12421,11 +12836,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A3:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12436,7 +12851,15 @@
     <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
       <c r="B4" t="s">
         <v>630</v>
       </c>
@@ -12444,37 +12867,45 @@
         <v>631</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
       <c r="B9" t="s">
         <v>635</v>
       </c>
       <c r="C9" t="s">
         <v>636</v>
       </c>
-      <c r="E9" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
         <v>637</v>
       </c>
-      <c r="F9" t="s">
+      <c r="C11" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F10" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
         <v>638</v>
       </c>
     </row>
@@ -12485,18 +12916,18 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" style="98" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" style="82" customWidth="1"/>
     <col min="3" max="4" width="19.109375" style="54" customWidth="1"/>
     <col min="5" max="6" width="15.33203125" style="54" customWidth="1"/>
     <col min="7" max="7" width="25.88671875" style="54" customWidth="1"/>
@@ -12561,10 +12992,10 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="83" t="s">
         <v>654</v>
       </c>
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="82" t="s">
         <v>743</v>
       </c>
       <c r="I2" s="54" t="s">
@@ -12593,8 +13024,8 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
-      <c r="B3" s="98" t="s">
+      <c r="A3" s="83"/>
+      <c r="B3" s="82" t="s">
         <v>742</v>
       </c>
       <c r="I3" s="54" t="s">
@@ -12617,8 +13048,8 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="99"/>
-      <c r="B4" s="98" t="s">
+      <c r="A4" s="83"/>
+      <c r="B4" s="82" t="s">
         <v>741</v>
       </c>
       <c r="I4" s="54" t="s">
@@ -12641,10 +13072,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="83" t="s">
         <v>715</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="82" t="s">
         <v>311</v>
       </c>
       <c r="G5" s="54" t="s">
@@ -12667,8 +13098,8 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="99"/>
-      <c r="B6" s="98" t="s">
+      <c r="A6" s="83"/>
+      <c r="B6" s="82" t="s">
         <v>312</v>
       </c>
       <c r="I6" s="54" t="s">
@@ -12685,8 +13116,8 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="99"/>
-      <c r="B7" s="98" t="s">
+      <c r="A7" s="83"/>
+      <c r="B7" s="82" t="s">
         <v>441</v>
       </c>
       <c r="I7" s="54" t="s">
@@ -12703,8 +13134,8 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="99"/>
-      <c r="B8" s="98" t="s">
+      <c r="A8" s="83"/>
+      <c r="B8" s="82" t="s">
         <v>716</v>
       </c>
       <c r="I8" s="54" t="s">
@@ -12721,26 +13152,26 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="83" t="s">
         <v>765</v>
       </c>
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="82" t="s">
         <v>766</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="99" t="s">
+      <c r="A10" s="83" t="s">
         <v>767</v>
       </c>
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="82" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="85" t="s">
         <v>734</v>
       </c>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="82" t="s">
         <v>739</v>
       </c>
       <c r="C11" s="54" t="s">
@@ -12760,10 +13191,10 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="99" t="s">
+      <c r="A12" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="82" t="s">
         <v>378</v>
       </c>
       <c r="G12" s="46" t="s">
@@ -12786,7 +13217,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="99" t="s">
+      <c r="A13" s="83" t="s">
         <v>655</v>
       </c>
       <c r="B13" s="77" t="s">
@@ -12815,10 +13246,10 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="99" t="s">
+      <c r="A14" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="82" t="s">
         <v>653</v>
       </c>
       <c r="G14" s="46"/>
@@ -12842,7 +13273,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="99"/>
+      <c r="A15" s="83"/>
       <c r="B15" s="77" t="s">
         <v>427</v>
       </c>
@@ -12872,10 +13303,10 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="99" t="s">
+      <c r="A16" s="83" t="s">
         <v>648</v>
       </c>
-      <c r="B16" s="98" t="s">
+      <c r="B16" s="82" t="s">
         <v>409</v>
       </c>
       <c r="G16" s="46" t="s">
@@ -12907,10 +13338,10 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="99" t="s">
+      <c r="A17" s="83" t="s">
         <v>649</v>
       </c>
-      <c r="B17" s="98" t="s">
+      <c r="B17" s="82" t="s">
         <v>372</v>
       </c>
       <c r="G17" s="46" t="s">
@@ -12942,10 +13373,10 @@
       </c>
     </row>
     <row r="18" spans="1:17" ht="27" x14ac:dyDescent="0.3">
-      <c r="A18" s="99" t="s">
+      <c r="A18" s="83" t="s">
         <v>687</v>
       </c>
-      <c r="B18" s="98" t="s">
+      <c r="B18" s="82" t="s">
         <v>680</v>
       </c>
       <c r="C18" s="54" t="s">
@@ -12983,10 +13414,10 @@
       </c>
     </row>
     <row r="19" spans="1:17" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A19" s="99" t="s">
+      <c r="A19" s="83" t="s">
         <v>688</v>
       </c>
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="82" t="s">
         <v>679</v>
       </c>
       <c r="C19" s="54" t="s">
@@ -13021,10 +13452,10 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="99" t="s">
+      <c r="A20" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="98" t="s">
+      <c r="B20" s="82" t="s">
         <v>652</v>
       </c>
       <c r="H20" s="54" t="s">
@@ -13059,10 +13490,10 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="99" t="s">
+      <c r="A21" s="83" t="s">
         <v>392</v>
       </c>
-      <c r="B21" s="98" t="s">
+      <c r="B21" s="82" t="s">
         <v>606</v>
       </c>
       <c r="G21" s="65" t="s">
@@ -13088,7 +13519,7 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="99" t="s">
+      <c r="A22" s="83" t="s">
         <v>609</v>
       </c>
       <c r="B22" s="77" t="s">
@@ -13117,7 +13548,7 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" s="99" t="s">
+      <c r="A23" s="83" t="s">
         <v>621</v>
       </c>
       <c r="B23" s="77" t="s">
@@ -13146,10 +13577,10 @@
       </c>
     </row>
     <row r="24" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="99" t="s">
+      <c r="A24" s="83" t="s">
         <v>671</v>
       </c>
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="82" t="s">
         <v>668</v>
       </c>
       <c r="C24" s="54" t="s">
@@ -13190,10 +13621,10 @@
       </c>
     </row>
     <row r="25" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="99" t="s">
+      <c r="A25" s="83" t="s">
         <v>672</v>
       </c>
-      <c r="B25" s="98" t="s">
+      <c r="B25" s="82" t="s">
         <v>670</v>
       </c>
       <c r="C25" s="54" t="s">
@@ -13234,8 +13665,8 @@
       </c>
     </row>
     <row r="26" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="99"/>
-      <c r="B26" s="98" t="s">
+      <c r="A26" s="83"/>
+      <c r="B26" s="82" t="s">
         <v>669</v>
       </c>
       <c r="G26" s="54" t="s">
@@ -13270,7 +13701,7 @@
       </c>
     </row>
     <row r="27" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="99" t="s">
+      <c r="A27" s="83" t="s">
         <v>666</v>
       </c>
       <c r="B27" s="77" t="s">
@@ -13299,7 +13730,7 @@
       </c>
     </row>
     <row r="28" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="99" t="s">
+      <c r="A28" s="83" t="s">
         <v>366</v>
       </c>
       <c r="B28" s="77" t="s">
@@ -13328,7 +13759,7 @@
       </c>
     </row>
     <row r="29" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="99" t="s">
+      <c r="A29" s="83" t="s">
         <v>691</v>
       </c>
       <c r="B29" s="77" t="s">
@@ -13363,7 +13794,7 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A30" s="99" t="s">
+      <c r="A30" s="83" t="s">
         <v>664</v>
       </c>
       <c r="B30" s="77" t="s">
@@ -13392,7 +13823,7 @@
       </c>
     </row>
     <row r="31" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="99" t="s">
+      <c r="A31" s="83" t="s">
         <v>712</v>
       </c>
       <c r="B31" s="77" t="s">
@@ -13413,7 +13844,7 @@
       </c>
     </row>
     <row r="32" spans="1:17" ht="72" x14ac:dyDescent="0.3">
-      <c r="A32" s="99" t="s">
+      <c r="A32" s="83" t="s">
         <v>708</v>
       </c>
       <c r="B32" s="77" t="s">
@@ -13440,7 +13871,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" ht="72" x14ac:dyDescent="0.3">
-      <c r="A33" s="99"/>
+      <c r="A33" s="83"/>
       <c r="B33" s="77" t="s">
         <v>710</v>
       </c>
@@ -13462,10 +13893,10 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34" s="99" t="s">
+      <c r="A34" s="83" t="s">
         <v>675</v>
       </c>
-      <c r="B34" s="98" t="s">
+      <c r="B34" s="82" t="s">
         <v>423</v>
       </c>
       <c r="G34" s="54" t="s">
@@ -13497,7 +13928,7 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A35" s="100" t="s">
+      <c r="A35" s="84" t="s">
         <v>365</v>
       </c>
       <c r="B35" s="77" t="s">
@@ -13534,8 +13965,8 @@
       </c>
     </row>
     <row r="36" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="99"/>
-      <c r="B36" s="98" t="s">
+      <c r="A36" s="83"/>
+      <c r="B36" s="82" t="s">
         <v>677</v>
       </c>
       <c r="I36" s="54" t="s">
@@ -13555,8 +13986,8 @@
       </c>
     </row>
     <row r="37" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="99"/>
-      <c r="B37" s="98" t="s">
+      <c r="A37" s="83"/>
+      <c r="B37" s="82" t="s">
         <v>382</v>
       </c>
       <c r="I37" s="54" t="s">
@@ -13573,8 +14004,8 @@
       </c>
     </row>
     <row r="38" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="99"/>
-      <c r="B38" s="98" t="s">
+      <c r="A38" s="83"/>
+      <c r="B38" s="82" t="s">
         <v>678</v>
       </c>
       <c r="I38" s="54" t="s">
@@ -13591,10 +14022,10 @@
       </c>
     </row>
     <row r="39" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="101" t="s">
+      <c r="A39" s="85" t="s">
         <v>681</v>
       </c>
-      <c r="B39" s="98" t="s">
+      <c r="B39" s="82" t="s">
         <v>738</v>
       </c>
       <c r="C39" s="54" t="s">
@@ -13635,8 +14066,8 @@
       </c>
     </row>
     <row r="40" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="99"/>
-      <c r="B40" s="98" t="s">
+      <c r="A40" s="83"/>
+      <c r="B40" s="82" t="s">
         <v>444</v>
       </c>
       <c r="G40" s="54" t="s">
@@ -13659,10 +14090,10 @@
       </c>
     </row>
     <row r="41" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="99" t="s">
+      <c r="A41" s="83" t="s">
         <v>701</v>
       </c>
-      <c r="B41" s="98" t="s">
+      <c r="B41" s="82" t="s">
         <v>683</v>
       </c>
       <c r="I41" s="54" t="s">
@@ -13679,8 +14110,8 @@
       </c>
     </row>
     <row r="42" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="99"/>
-      <c r="B42" s="98" t="s">
+      <c r="A42" s="83"/>
+      <c r="B42" s="82" t="s">
         <v>684</v>
       </c>
       <c r="I42" s="54" t="s">
@@ -13694,8 +14125,8 @@
       </c>
     </row>
     <row r="43" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="99"/>
-      <c r="B43" s="98" t="s">
+      <c r="A43" s="83"/>
+      <c r="B43" s="82" t="s">
         <v>685</v>
       </c>
       <c r="I43" s="54" t="s">
@@ -13712,8 +14143,8 @@
       </c>
     </row>
     <row r="44" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="99"/>
-      <c r="B44" s="98" t="s">
+      <c r="A44" s="83"/>
+      <c r="B44" s="82" t="s">
         <v>686</v>
       </c>
       <c r="I44" s="54" t="s">
@@ -13730,8 +14161,8 @@
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A45" s="99"/>
-      <c r="B45" s="98" t="s">
+      <c r="A45" s="83"/>
+      <c r="B45" s="82" t="s">
         <v>449</v>
       </c>
       <c r="G45" s="54" t="s">
@@ -13763,8 +14194,8 @@
       </c>
     </row>
     <row r="46" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="99"/>
-      <c r="B46" s="98" t="s">
+      <c r="A46" s="83"/>
+      <c r="B46" s="82" t="s">
         <v>706</v>
       </c>
       <c r="C46" s="54" t="s">
@@ -13799,8 +14230,8 @@
       </c>
     </row>
     <row r="47" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="99"/>
-      <c r="B47" s="98" t="s">
+      <c r="A47" s="83"/>
+      <c r="B47" s="82" t="s">
         <v>707</v>
       </c>
       <c r="C47" s="54" t="s">
@@ -13835,10 +14266,10 @@
       </c>
     </row>
     <row r="48" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="99" t="s">
+      <c r="A48" s="83" t="s">
         <v>455</v>
       </c>
-      <c r="B48" s="98" t="s">
+      <c r="B48" s="82" t="s">
         <v>689</v>
       </c>
       <c r="C48" s="54" t="s">
@@ -13873,10 +14304,10 @@
       </c>
     </row>
     <row r="49" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="99" t="s">
+      <c r="A49" s="83" t="s">
         <v>453</v>
       </c>
-      <c r="B49" s="98" t="s">
+      <c r="B49" s="82" t="s">
         <v>690</v>
       </c>
       <c r="C49" s="54" t="s">
@@ -13911,10 +14342,10 @@
       </c>
     </row>
     <row r="50" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="99" t="s">
+      <c r="A50" s="83" t="s">
         <v>702</v>
       </c>
-      <c r="B50" s="98" t="s">
+      <c r="B50" s="82" t="s">
         <v>699</v>
       </c>
       <c r="C50" s="54" t="s">
@@ -13952,10 +14383,10 @@
       </c>
     </row>
     <row r="51" spans="1:17" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="99" t="s">
+      <c r="A51" s="83" t="s">
         <v>703</v>
       </c>
-      <c r="B51" s="98" t="s">
+      <c r="B51" s="82" t="s">
         <v>700</v>
       </c>
       <c r="C51" s="54" t="s">
@@ -13993,10 +14424,10 @@
       </c>
     </row>
     <row r="52" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="99" t="s">
+      <c r="A52" s="83" t="s">
         <v>694</v>
       </c>
-      <c r="B52" s="98" t="s">
+      <c r="B52" s="82" t="s">
         <v>693</v>
       </c>
       <c r="G52" s="54" t="s">
@@ -14034,10 +14465,10 @@
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A53" s="99" t="s">
+      <c r="A53" s="83" t="s">
         <v>713</v>
       </c>
-      <c r="B53" s="98" t="s">
+      <c r="B53" s="82" t="s">
         <v>705</v>
       </c>
       <c r="C53" s="54" t="s">
@@ -14078,10 +14509,10 @@
       </c>
     </row>
     <row r="54" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="101" t="s">
+      <c r="A54" s="85" t="s">
         <v>732</v>
       </c>
-      <c r="B54" s="98" t="s">
+      <c r="B54" s="82" t="s">
         <v>761</v>
       </c>
       <c r="C54" s="54" t="s">
@@ -14116,10 +14547,10 @@
       </c>
     </row>
     <row r="55" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A55" s="102" t="s">
+      <c r="A55" s="86" t="s">
         <v>759</v>
       </c>
-      <c r="B55" s="98" t="s">
+      <c r="B55" s="82" t="s">
         <v>762</v>
       </c>
       <c r="C55" s="54" t="s">
@@ -14151,10 +14582,10 @@
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A56" s="101" t="s">
+      <c r="A56" s="85" t="s">
         <v>758</v>
       </c>
-      <c r="B56" s="98" t="s">
+      <c r="B56" s="82" t="s">
         <v>763</v>
       </c>
       <c r="C56" s="54" t="s">
@@ -14186,10 +14617,10 @@
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A57" s="101" t="s">
+      <c r="A57" s="85" t="s">
         <v>757</v>
       </c>
-      <c r="B57" s="98" t="s">
+      <c r="B57" s="82" t="s">
         <v>764</v>
       </c>
       <c r="C57" s="54" t="s">
@@ -14221,10 +14652,10 @@
       </c>
     </row>
     <row r="58" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="101" t="s">
+      <c r="A58" s="85" t="s">
         <v>756</v>
       </c>
-      <c r="B58" s="98" t="s">
+      <c r="B58" s="82" t="s">
         <v>769</v>
       </c>
       <c r="C58" s="54" t="s">
@@ -14256,10 +14687,10 @@
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A59" s="101" t="s">
+      <c r="A59" s="85" t="s">
         <v>760</v>
       </c>
-      <c r="B59" s="98" t="s">
+      <c r="B59" s="82" t="s">
         <v>770</v>
       </c>
       <c r="C59" s="54" t="s">
@@ -14291,10 +14722,10 @@
       </c>
     </row>
     <row r="60" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="101" t="s">
+      <c r="A60" s="85" t="s">
         <v>755</v>
       </c>
-      <c r="B60" s="98" t="s">
+      <c r="B60" s="82" t="s">
         <v>771</v>
       </c>
       <c r="C60" s="54" t="s">
@@ -14326,7 +14757,7 @@
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A61" s="102" t="s">
+      <c r="A61" s="86" t="s">
         <v>754</v>
       </c>
       <c r="C61" s="54" t="s">
@@ -14358,7 +14789,7 @@
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A62" s="101" t="s">
+      <c r="A62" s="85" t="s">
         <v>753</v>
       </c>
       <c r="C62" s="54" t="s">
@@ -14390,10 +14821,10 @@
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A63" s="101" t="s">
+      <c r="A63" s="85" t="s">
         <v>463</v>
       </c>
-      <c r="B63" s="98" t="s">
+      <c r="B63" s="82" t="s">
         <v>750</v>
       </c>
       <c r="C63" s="54" t="s">
@@ -14442,10 +14873,10 @@
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A64" s="101" t="s">
+      <c r="A64" s="85" t="s">
         <v>624</v>
       </c>
-      <c r="B64" s="98" t="s">
+      <c r="B64" s="82" t="s">
         <v>751</v>
       </c>
       <c r="C64" s="54" t="s">
@@ -14484,10 +14915,10 @@
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A65" s="101" t="s">
+      <c r="A65" s="85" t="s">
         <v>733</v>
       </c>
-      <c r="B65" s="98" t="s">
+      <c r="B65" s="82" t="s">
         <v>752</v>
       </c>
       <c r="C65" s="54" t="s">
@@ -14535,10 +14966,10 @@
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A66" s="101" t="s">
+      <c r="A66" s="85" t="s">
         <v>722</v>
       </c>
-      <c r="B66" s="98" t="s">
+      <c r="B66" s="82" t="s">
         <v>717</v>
       </c>
       <c r="C66" s="54" t="s">
@@ -14580,10 +15011,10 @@
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A67" s="99" t="s">
+      <c r="A67" s="83" t="s">
         <v>721</v>
       </c>
-      <c r="B67" s="98" t="s">
+      <c r="B67" s="82" t="s">
         <v>719</v>
       </c>
       <c r="C67" s="54" t="s">
@@ -14628,10 +15059,10 @@
       </c>
     </row>
     <row r="68" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="101" t="s">
+      <c r="A68" s="85" t="s">
         <v>724</v>
       </c>
-      <c r="B68" s="98" t="s">
+      <c r="B68" s="82" t="s">
         <v>727</v>
       </c>
       <c r="C68" s="54" t="s">
@@ -14673,10 +15104,10 @@
       </c>
     </row>
     <row r="69" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="101" t="s">
+      <c r="A69" s="85" t="s">
         <v>725</v>
       </c>
-      <c r="B69" s="98" t="s">
+      <c r="B69" s="82" t="s">
         <v>727</v>
       </c>
       <c r="C69" s="54" t="s">
@@ -14718,10 +15149,10 @@
       </c>
     </row>
     <row r="70" spans="1:17" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="101" t="s">
+      <c r="A70" s="85" t="s">
         <v>723</v>
       </c>
-      <c r="B70" s="98" t="s">
+      <c r="B70" s="82" t="s">
         <v>720</v>
       </c>
       <c r="C70" s="54" t="s">
@@ -14766,7 +15197,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P70"/>
+  <autoFilter ref="A1:P70" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <conditionalFormatting sqref="A1:A9 A57:A70 A11:A55">
     <cfRule type="containsBlanks" dxfId="1" priority="3">
       <formula>LEN(TRIM(A1))=0</formula>
@@ -14778,25 +15209,25 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K5" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>"Datetime,Categorical,Numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>"Input,Output,Calculated"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>"R,NR"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:O1048576">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:O1048576" xr:uid="{00000000-0002-0000-0700-000003000000}">
       <formula1>"0,1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{00000000-0002-0000-0700-000004000000}">
       <formula1>"General,PD,LGD,CCF,ELBE,LGDD,SL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0700-000005000000}">
       <formula1>"create_data_set,model,Run_reporting_tool,Validation_tests,export,visualisation_dash"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K1048576" xr:uid="{00000000-0002-0000-0700-000006000000}">
       <formula1>"Datetime,Categorical,Numeric,Dataframe"</formula1>
     </dataValidation>
   </dataValidations>
@@ -14808,389 +15239,629 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:D25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A243D83-5EB1-4694-8D19-362C751CED51}">
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="31" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="31"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
-        <v>562</v>
-      </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="88"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="89"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="91"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="82" t="s">
-        <v>563</v>
-      </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="84"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
-        <v>564</v>
-      </c>
-      <c r="B5" s="92" t="s">
-        <v>565</v>
-      </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="94"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
-        <v>566</v>
-      </c>
-      <c r="B6" s="92" t="s">
-        <v>567</v>
-      </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="94"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
-        <v>568</v>
-      </c>
-      <c r="B7" s="95" t="s">
-        <v>569</v>
-      </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="97"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="34" t="s">
-        <v>570</v>
-      </c>
-      <c r="B8" s="95" t="s">
-        <v>571</v>
-      </c>
-      <c r="C8" s="96"/>
-      <c r="D8" s="97"/>
-    </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="82" t="s">
-        <v>572</v>
-      </c>
-      <c r="B10" s="83"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="84"/>
-    </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
-        <v>573</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>574</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>575</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32" t="s">
-        <v>576</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>577</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>578</v>
-      </c>
-      <c r="D12" s="35" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="32" t="s">
-        <v>580</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>581</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>582</v>
-      </c>
-      <c r="D13" s="35" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="33" t="s">
-        <v>584</v>
-      </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-    </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="33"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-    </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="85" t="s">
-        <v>585</v>
-      </c>
-      <c r="B17" s="85"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="85"/>
-    </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>590</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>594</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>598</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>605</v>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="103" t="s">
+        <v>772</v>
+      </c>
+      <c r="B1" s="103" t="s">
+        <v>356</v>
+      </c>
+      <c r="C1" s="103" t="s">
+        <v>357</v>
+      </c>
+      <c r="D1" s="103" t="s">
+        <v>796</v>
+      </c>
+      <c r="E1" s="103" t="s">
+        <v>784</v>
+      </c>
+      <c r="F1" s="103" t="s">
+        <v>794</v>
+      </c>
+      <c r="G1" s="103" t="s">
+        <v>807</v>
+      </c>
+      <c r="H1" s="103" t="s">
+        <v>808</v>
+      </c>
+      <c r="I1" s="103" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D2" t="s">
+        <v>774</v>
+      </c>
+      <c r="E2" t="s">
+        <v>729</v>
+      </c>
+      <c r="F2" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G2" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="H2" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="I2" s="54" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C3" t="s">
+        <v>624</v>
+      </c>
+      <c r="D3" t="s">
+        <v>773</v>
+      </c>
+      <c r="E3" t="s">
+        <v>729</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G3" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C4" t="s">
+        <v>775</v>
+      </c>
+      <c r="D4" t="s">
+        <v>785</v>
+      </c>
+      <c r="E4" t="s">
+        <v>729</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G4" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="H4" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="I4" s="54" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C5" t="s">
+        <v>776</v>
+      </c>
+      <c r="D5" t="s">
+        <v>786</v>
+      </c>
+      <c r="E5" t="s">
+        <v>729</v>
+      </c>
+      <c r="F5" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G5" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="H5" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="I5" s="54" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C6" t="s">
+        <v>392</v>
+      </c>
+      <c r="D6" t="s">
+        <v>777</v>
+      </c>
+      <c r="E6" t="s">
+        <v>729</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="H6" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="I6" s="54" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B7" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C7" t="s">
+        <v>725</v>
+      </c>
+      <c r="D7" t="s">
+        <v>787</v>
+      </c>
+      <c r="E7" t="s">
+        <v>731</v>
+      </c>
+      <c r="F7" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G7" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H7" s="54" t="s">
+        <v>810</v>
+      </c>
+      <c r="I7" s="54" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C8" t="s">
+        <v>778</v>
+      </c>
+      <c r="D8" t="s">
+        <v>788</v>
+      </c>
+      <c r="E8" t="s">
+        <v>731</v>
+      </c>
+      <c r="F8" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H8" s="54" t="s">
+        <v>810</v>
+      </c>
+      <c r="I8" s="54" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C9" t="s">
+        <v>724</v>
+      </c>
+      <c r="D9" t="s">
+        <v>790</v>
+      </c>
+      <c r="E9" t="s">
+        <v>731</v>
+      </c>
+      <c r="F9" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G9" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H9" s="54" t="s">
+        <v>810</v>
+      </c>
+      <c r="I9" s="54" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C10" t="s">
+        <v>779</v>
+      </c>
+      <c r="D10" t="s">
+        <v>789</v>
+      </c>
+      <c r="E10" t="s">
+        <v>731</v>
+      </c>
+      <c r="F10" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H10" s="54" t="s">
+        <v>810</v>
+      </c>
+      <c r="I10" s="54" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B11" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C11" t="s">
+        <v>780</v>
+      </c>
+      <c r="D11" t="s">
+        <v>791</v>
+      </c>
+      <c r="E11" t="s">
+        <v>731</v>
+      </c>
+      <c r="F11" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>809</v>
+      </c>
+      <c r="I11" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C12" t="s">
+        <v>781</v>
+      </c>
+      <c r="D12" t="s">
+        <v>792</v>
+      </c>
+      <c r="E12" t="s">
+        <v>731</v>
+      </c>
+      <c r="F12" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G12" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H12" s="54" t="s">
+        <v>809</v>
+      </c>
+      <c r="I12" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C13" t="s">
+        <v>803</v>
+      </c>
+      <c r="D13" t="s">
+        <v>804</v>
+      </c>
+      <c r="E13" t="s">
+        <v>731</v>
+      </c>
+      <c r="F13" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G13" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H13" s="54" t="s">
+        <v>809</v>
+      </c>
+      <c r="I13" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B14" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C14" t="s">
+        <v>782</v>
+      </c>
+      <c r="D14" t="s">
+        <v>802</v>
+      </c>
+      <c r="E14" t="s">
+        <v>731</v>
+      </c>
+      <c r="F14" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G14" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H14" s="54" t="s">
+        <v>809</v>
+      </c>
+      <c r="I14" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C15" t="s">
+        <v>783</v>
+      </c>
+      <c r="D15" t="s">
+        <v>793</v>
+      </c>
+      <c r="E15" t="s">
+        <v>731</v>
+      </c>
+      <c r="F15" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G15" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H15" s="54" t="s">
+        <v>809</v>
+      </c>
+      <c r="I15" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C16" t="s">
+        <v>780</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>797</v>
+      </c>
+      <c r="E16" t="s">
+        <v>731</v>
+      </c>
+      <c r="F16" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G16" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H16" t="s">
+        <v>798</v>
+      </c>
+      <c r="I16" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C17" t="s">
+        <v>781</v>
+      </c>
+      <c r="D17" s="54" t="s">
+        <v>799</v>
+      </c>
+      <c r="E17" t="s">
+        <v>731</v>
+      </c>
+      <c r="F17" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G17" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H17" t="s">
+        <v>798</v>
+      </c>
+      <c r="I17" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C18" t="s">
+        <v>803</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>800</v>
+      </c>
+      <c r="E18" t="s">
+        <v>731</v>
+      </c>
+      <c r="F18" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G18" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H18" t="s">
+        <v>798</v>
+      </c>
+      <c r="I18" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B19" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C19" t="s">
+        <v>782</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>801</v>
+      </c>
+      <c r="E19" t="s">
+        <v>731</v>
+      </c>
+      <c r="F19" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G19" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H19" t="s">
+        <v>798</v>
+      </c>
+      <c r="I19" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B20" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C20" t="s">
+        <v>783</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>805</v>
+      </c>
+      <c r="E20" t="s">
+        <v>731</v>
+      </c>
+      <c r="F20" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G20" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H20" t="s">
+        <v>798</v>
+      </c>
+      <c r="I20" t="s">
+        <v>813</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A20" xr:uid="{8D76983D-28D8-40FA-81DF-50E84AF004E2}">
+      <formula1>"Input,Output,Calculated"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F20" xr:uid="{5A23AC18-18EC-4ADD-813B-C42B62155790}">
+      <formula1>"Datetime,Categorical,Numeric"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B20" xr:uid="{0603A4C1-7DAA-44AA-8103-97FDFBDD8906}">
+      <formula1>"General,PD,LGD,CCF,ELBE,LGDD,SL"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Z:\FSO Advisory All\2. FSO Advisory _ Solutions\3. Risk\2. Data Quality\1. Conceptual\[DataQuality_Testing_Conceptual.xlsb]Lists'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C12:D13</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="33ef62f9-2e07-484b-bd79-00aec90129fe" ContentTypeId="0x010100826318CDA76982469C2C3CD2CD5847410101" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <jc981bd8ab5b47fd91abb7684c0f405b xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Brussels</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0086b60c-6752-48fa-8e91-a8805d8608ed</TermId>
-        </TermInfo>
-      </Terms>
-    </jc981bd8ab5b47fd91abb7684c0f405b>
-    <i14ea8bbd518495ea0e20ac1ad18c527 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Campaign Materials</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10e3cb14-f0bd-4a0a-bb1a-58c7e26fd5e4</TermId>
-        </TermInfo>
-      </Terms>
-    </i14ea8bbd518495ea0e20ac1ad18c527>
-    <b4187e12891e46deb4d240a4b28bdb90 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b4187e12891e46deb4d240a4b28bdb90>
-    <TaxCatchAll xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Value>13</Value>
-      <Value>12</Value>
-      <Value>11</Value>
-    </TaxCatchAll>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <e0e024ccac5240e69ae9c38a41bfa7a5 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </e0e024ccac5240e69ae9c38a41bfa7a5>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <Classification_x0020_Status xmlns="35818088-e62d-4edf-bbb6-409430aef268" xsi:nil="true"/>
-    <k8128b1c45734e36a24fce652bc7ffb7 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Quantitative Services</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8ac922a9-ccce-4035-83d6-3ab1113bed22</TermId>
-        </TermInfo>
-      </Terms>
-    </k8128b1c45734e36a24fce652bc7ffb7>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-    <_dlc_DocId xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">3KSVPJYEA2AR-1011915566-26</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
-      <Url>https://sites.ey.com/sites/QAS_BELGIUM/_layouts/15/DocIdRedir.aspx?ID=3KSVPJYEA2AR-1011915566-26</Url>
-      <Description>3KSVPJYEA2AR-1011915566-26</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
-      <UserInfo>
-        <DisplayName>Diego De Plaen</DisplayName>
-        <AccountId>56</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Antonio Millan Puebla</DisplayName>
-        <AccountId>31</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sander Vandevenne</DisplayName>
-        <AccountId>54</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="EY Collaboration Document" ma:contentTypeID="0x010100826318CDA76982469C2C3CD2CD58474101010039A9718220E30744AB05D9570037D8A1" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0a3d079c8d19385a693d7ea59f238e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="50c908b1-f277-4340-90a9-4611d0b0f078" xmlns:ns4="35818088-e62d-4edf-bbb6-409430aef268" xmlns:ns5="40c6704c-f77c-4b8a-96a1-a10a2e12c42b" xmlns:ns6="96860b88-8044-411d-9267-72f1d28f5ec3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0684eb5fe437c3d422fbfa93671a941" ns1:_="" ns2:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15535,9 +16206,94 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <jc981bd8ab5b47fd91abb7684c0f405b xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Brussels</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0086b60c-6752-48fa-8e91-a8805d8608ed</TermId>
+        </TermInfo>
+      </Terms>
+    </jc981bd8ab5b47fd91abb7684c0f405b>
+    <i14ea8bbd518495ea0e20ac1ad18c527 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Campaign Materials</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10e3cb14-f0bd-4a0a-bb1a-58c7e26fd5e4</TermId>
+        </TermInfo>
+      </Terms>
+    </i14ea8bbd518495ea0e20ac1ad18c527>
+    <b4187e12891e46deb4d240a4b28bdb90 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b4187e12891e46deb4d240a4b28bdb90>
+    <TaxCatchAll xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Value>13</Value>
+      <Value>12</Value>
+      <Value>11</Value>
+    </TaxCatchAll>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <e0e024ccac5240e69ae9c38a41bfa7a5 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e0e024ccac5240e69ae9c38a41bfa7a5>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <Classification_x0020_Status xmlns="35818088-e62d-4edf-bbb6-409430aef268" xsi:nil="true"/>
+    <k8128b1c45734e36a24fce652bc7ffb7 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Quantitative Services</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8ac922a9-ccce-4035-83d6-3ab1113bed22</TermId>
+        </TermInfo>
+      </Terms>
+    </k8128b1c45734e36a24fce652bc7ffb7>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+    <_dlc_DocId xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">3KSVPJYEA2AR-1011915566-26</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
+      <Url>https://sites.ey.com/sites/QAS_BELGIUM/_layouts/15/DocIdRedir.aspx?ID=3KSVPJYEA2AR-1011915566-26</Url>
+      <Description>3KSVPJYEA2AR-1011915566-26</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
+      <UserInfo>
+        <DisplayName>Diego De Plaen</DisplayName>
+        <AccountId>56</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Antonio Millan Puebla</DisplayName>
+        <AccountId>31</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sander Vandevenne</DisplayName>
+        <AccountId>54</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="33ef62f9-2e07-484b-bd79-00aec90129fe" ContentTypeId="0x010100826318CDA76982469C2C3CD2CD5847410101" PreviousValue="false"/>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15591,34 +16347,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D6130A-D52D-416E-88B9-F6885590E854}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4AB6DE9-C584-4E87-8FF5-1A82C035629B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A2966CE-FBFB-42D6-8AF5-4361359F35A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="50c908b1-f277-4340-90a9-4611d0b0f078"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="35818088-e62d-4edf-bbb6-409430aef268"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="96860b88-8044-411d-9267-72f1d28f5ec3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="40c6704c-f77c-4b8a-96a1-a10a2e12c42b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2D0B982-DBCA-4EED-A652-6CD257CDA216}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15640,10 +16376,30 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A2966CE-FBFB-42D6-8AF5-4361359F35A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="50c908b1-f277-4340-90a9-4611d0b0f078"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="35818088-e62d-4edf-bbb6-409430aef268"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="96860b88-8044-411d-9267-72f1d28f5ec3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="40c6704c-f77c-4b8a-96a1-a10a2e12c42b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4AB6DE9-C584-4E87-8FF5-1A82C035629B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D6130A-D52D-416E-88B9-F6885590E854}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Jeffrey test according to gAUC_LGD template
</commit_message>
<xml_diff>
--- a/IRB models/Data Model.xlsx
+++ b/IRB models/Data Model.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bebxadvboey\Documents\Python\GitHub\ML4Credit\IRB models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bebxadvsven\Documents\Python\GitHub\ML4Credit\IRB models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1F508E75-2F51-489E-9856-8A8D22AC95EC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" state="hidden" r:id="rId1"/>
@@ -33,7 +32,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
-  <calcPr calcId="179017" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="171027" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -43,12 +42,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sander Vandevenne</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -152,7 +151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -182,12 +181,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Brent Oeyen</author>
   </authors>
   <commentList>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
+    <comment ref="B11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -216,12 +215,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sander Vandevenne</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000002000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -269,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000003000000}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -294,7 +293,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000004000000}">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -318,7 +317,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000005000000}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -342,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000006000000}">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -366,7 +365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000007000000}">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -390,7 +389,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000008000000}">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -414,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000009000000}">
+    <comment ref="H23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -443,8 +442,93 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sander Vandevenne</author>
+  </authors>
+  <commentList>
+    <comment ref="C22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sander Vandevenne:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Should be unique</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C24" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sander Vandevenne:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This should be unique: How to cope with Default_binary serving as an input to multiple other 'technical names'?
+Note that previously the idea was captured by the 'precedent(s)' and dependent(s)' columns.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sander Vandevenne:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The grade and portfolio 'names' are duplicated information. In general, how to handle: 
+1. The same output needed to be reported at multiple instances (e.g. across parameter templates).
+2. Calculated or input 'technical' names that serve as input to multiple parameters </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="837">
   <si>
     <t>LoanStatNew</t>
   </si>
@@ -2934,11 +3018,86 @@
   <si>
     <t>LGD_toExcel</t>
   </si>
+  <si>
+    <t>PD_toExcel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 3.0      cell: D6 &amp; Range(.[D8], .[D8].End(xlDown)) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 3.0      cell: E6 &amp;  Range(.[E8], .[E8].End(xlDown)) </t>
+  </si>
+  <si>
+    <t>name_rating_grades</t>
+  </si>
+  <si>
+    <t>averagePD_pergrade</t>
+  </si>
+  <si>
+    <t>nb_customer_pergrade</t>
+  </si>
+  <si>
+    <t>nb_default_pergrade</t>
+  </si>
+  <si>
+    <t>jeffrey_test_pval_pergrade</t>
+  </si>
+  <si>
+    <t>original_exposure_pergrade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 3.0      cell: F6 &amp;  Range(.[F8], .[F8].End(xlDown)) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 3.0      cell: G6 &amp; Range(.[G8], .[G8].End(xlDown)) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 3.0      cell: H6 &amp; Range(.[H8], .[H8].End(xlDown)) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 3.0      cell: I6 &amp; Range(.[I8], .[I8].End(xlDown)) </t>
+  </si>
+  <si>
+    <t>Section 2.5.1(a)</t>
+  </si>
+  <si>
+    <t>Section 2.5.3: Name of the rating grade</t>
+  </si>
+  <si>
+    <t>Section 2.5.3: PD at the beginning of the relevant observation period</t>
+  </si>
+  <si>
+    <t>Section 2.5.3: Number of customers</t>
+  </si>
+  <si>
+    <t>Section 2.5.3: Number of defaulted customers</t>
+  </si>
+  <si>
+    <t>Section 2.5.3: The p-value per rating grade infered from the bèta distribution</t>
+  </si>
+  <si>
+    <t>Section 2.5.3: The original exposure at the beginning of the relevant observation period.</t>
+  </si>
+  <si>
+    <t>No explicit definition found</t>
+  </si>
+  <si>
+    <t>PD_tests</t>
+  </si>
+  <si>
+    <t>Jeffrey</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3859,7 +4018,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4025,6 +4184,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="37" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4073,7 +4233,7 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="88">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6580,7 +6740,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -7241,7 +7401,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B57" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:B57">
     <sortState ref="A2:B61">
       <sortCondition ref="A1:A61"/>
     </sortState>
@@ -7260,7 +7420,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -7279,74 +7439,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="92" t="s">
         <v>562</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="93"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="94"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="94"/>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="96"/>
+      <c r="A2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="97"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="88" t="s">
         <v>563</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="89"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="90"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>564</v>
       </c>
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="98" t="s">
         <v>565</v>
       </c>
-      <c r="C5" s="98"/>
-      <c r="D5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="100"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>566</v>
       </c>
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="98" t="s">
         <v>567</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="99"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="100"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>568</v>
       </c>
-      <c r="B7" s="100" t="s">
+      <c r="B7" s="101" t="s">
         <v>569</v>
       </c>
-      <c r="C7" s="101"/>
-      <c r="D7" s="102"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="103"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
         <v>570</v>
       </c>
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="101" t="s">
         <v>571</v>
       </c>
-      <c r="C8" s="101"/>
-      <c r="D8" s="102"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="103"/>
     </row>
     <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="88" t="s">
         <v>572</v>
       </c>
-      <c r="B10" s="88"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="89"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="90"/>
     </row>
     <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
@@ -7406,12 +7566,12 @@
     </row>
     <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="90" t="s">
+      <c r="A17" s="91" t="s">
         <v>585</v>
       </c>
-      <c r="B17" s="90"/>
-      <c r="C17" s="90"/>
-      <c r="D17" s="90"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="91"/>
+      <c r="D17" s="91"/>
     </row>
     <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -7540,7 +7700,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Z:\FSO Advisory All\2. FSO Advisory _ Solutions\3. Risk\2. Data Quality\1. Conceptual\[DataQuality_Testing_Conceptual.xlsb]Lists'!#REF!</xm:f>
           </x14:formula1>
@@ -7553,7 +7713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -7572,7 +7732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B109"/>
   <sheetViews>
@@ -8450,7 +8610,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B89" xr:uid="{00000000-0009-0000-0000-000002000000}">
+  <autoFilter ref="A1:B89">
     <sortState ref="A2:B93">
       <sortCondition ref="A1:A93"/>
     </sortState>
@@ -8469,7 +8629,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -8567,7 +8727,7 @@
       <c r="B12" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B10" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A1:B10"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -8580,7 +8740,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5">
     <tabColor theme="4"/>
   </sheetPr>
@@ -9056,7 +9216,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K247"/>
   <sheetViews>
@@ -12818,7 +12978,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
       <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
         <mc:Choice Requires="x12ac">
           <x12ac:list>"{""a"",""b""}"</x12ac:list>
@@ -12836,7 +12996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12916,7 +13076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15197,7 +15357,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P70" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
+  <autoFilter ref="A1:P70"/>
   <conditionalFormatting sqref="A1:A9 A57:A70 A11:A55">
     <cfRule type="containsBlanks" dxfId="1" priority="3">
       <formula>LEN(TRIM(A1))=0</formula>
@@ -15209,25 +15369,25 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K5" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K5">
       <formula1>"Datetime,Categorical,Numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{00000000-0002-0000-0700-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576">
       <formula1>"Input,Output,Calculated"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{00000000-0002-0000-0700-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
       <formula1>"R,NR"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:O1048576" xr:uid="{00000000-0002-0000-0700-000003000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:O1048576">
       <formula1>"0,1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{00000000-0002-0000-0700-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
       <formula1>"General,PD,LGD,CCF,ELBE,LGDD,SL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0700-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>"create_data_set,model,Run_reporting_tool,Validation_tests,export,visualisation_dash"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K1048576" xr:uid="{00000000-0002-0000-0700-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K1048576">
       <formula1>"Datetime,Categorical,Numeric,Dataframe"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15239,11 +15399,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A243D83-5EB1-4694-8D19-362C751CED51}">
-  <dimension ref="A1:I20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15260,31 +15421,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="87" t="s">
         <v>772</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="87" t="s">
         <v>356</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="C1" s="87" t="s">
         <v>357</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="D1" s="87" t="s">
         <v>796</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="E1" s="87" t="s">
         <v>784</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="F1" s="87" t="s">
         <v>794</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="G1" s="87" t="s">
         <v>807</v>
       </c>
-      <c r="H1" s="103" t="s">
+      <c r="H1" s="87" t="s">
         <v>808</v>
       </c>
-      <c r="I1" s="103" t="s">
+      <c r="I1" s="87" t="s">
         <v>806</v>
       </c>
     </row>
@@ -15839,20 +16000,465 @@
         <v>813</v>
       </c>
     </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="54"/>
+      <c r="B21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B22" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="E22" s="104" t="str">
+        <f>$E$2</f>
+        <v>create_data_set</v>
+      </c>
+      <c r="F22" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G22" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="H22" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="I22" s="83" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="83" t="s">
+        <v>645</v>
+      </c>
+      <c r="B23" s="83" t="s">
+        <v>365</v>
+      </c>
+      <c r="C23" s="104" t="s">
+        <v>365</v>
+      </c>
+      <c r="D23" s="104" t="s">
+        <v>827</v>
+      </c>
+      <c r="E23" s="104" t="str">
+        <f>$E$2</f>
+        <v>create_data_set</v>
+      </c>
+      <c r="F23" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G23" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="H23" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="I23" s="83" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="83" t="s">
+        <v>645</v>
+      </c>
+      <c r="B24" s="83" t="s">
+        <v>365</v>
+      </c>
+      <c r="C24" s="104" t="s">
+        <v>392</v>
+      </c>
+      <c r="D24" s="104" t="s">
+        <v>777</v>
+      </c>
+      <c r="E24" s="104" t="s">
+        <v>729</v>
+      </c>
+      <c r="F24" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G24" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="H24" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="I24" s="83" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C25" t="s">
+        <v>817</v>
+      </c>
+      <c r="D25" s="104" t="s">
+        <v>828</v>
+      </c>
+      <c r="E25" t="s">
+        <v>731</v>
+      </c>
+      <c r="F25" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G25" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H25" s="83" t="s">
+        <v>835</v>
+      </c>
+      <c r="I25" s="83" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C26" t="s">
+        <v>818</v>
+      </c>
+      <c r="D26" s="104" t="s">
+        <v>829</v>
+      </c>
+      <c r="E26" t="s">
+        <v>731</v>
+      </c>
+      <c r="F26" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G26" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H26" s="83" t="s">
+        <v>835</v>
+      </c>
+      <c r="I26" s="83" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B27" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C27" t="s">
+        <v>819</v>
+      </c>
+      <c r="D27" s="104" t="s">
+        <v>830</v>
+      </c>
+      <c r="E27" t="s">
+        <v>731</v>
+      </c>
+      <c r="F27" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G27" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H27" s="83" t="s">
+        <v>835</v>
+      </c>
+      <c r="I27" s="83" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B28" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C28" t="s">
+        <v>820</v>
+      </c>
+      <c r="D28" s="104" t="s">
+        <v>831</v>
+      </c>
+      <c r="E28" t="s">
+        <v>731</v>
+      </c>
+      <c r="F28" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G28" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H28" s="83" t="s">
+        <v>835</v>
+      </c>
+      <c r="I28" s="83" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B29" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C29" t="s">
+        <v>821</v>
+      </c>
+      <c r="D29" s="104" t="s">
+        <v>832</v>
+      </c>
+      <c r="E29" t="s">
+        <v>731</v>
+      </c>
+      <c r="F29" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G29" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H29" s="83" t="s">
+        <v>835</v>
+      </c>
+      <c r="I29" s="83" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B30" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C30" t="s">
+        <v>822</v>
+      </c>
+      <c r="D30" s="104" t="s">
+        <v>833</v>
+      </c>
+      <c r="E30" t="s">
+        <v>731</v>
+      </c>
+      <c r="F30" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G30" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H30" s="83" t="s">
+        <v>835</v>
+      </c>
+      <c r="I30" s="83" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B31" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C31" t="s">
+        <v>817</v>
+      </c>
+      <c r="D31" t="s">
+        <v>815</v>
+      </c>
+      <c r="E31" t="s">
+        <v>731</v>
+      </c>
+      <c r="F31" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G31" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H31" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="I31" s="54" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B32" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C32" t="s">
+        <v>818</v>
+      </c>
+      <c r="D32" t="s">
+        <v>816</v>
+      </c>
+      <c r="E32" t="s">
+        <v>731</v>
+      </c>
+      <c r="F32" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G32" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H32" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="I32" s="54" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B33" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C33" t="s">
+        <v>819</v>
+      </c>
+      <c r="D33" t="s">
+        <v>823</v>
+      </c>
+      <c r="E33" t="s">
+        <v>731</v>
+      </c>
+      <c r="F33" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G33" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H33" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="I33" s="54" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B34" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C34" t="s">
+        <v>820</v>
+      </c>
+      <c r="D34" t="s">
+        <v>824</v>
+      </c>
+      <c r="E34" t="s">
+        <v>731</v>
+      </c>
+      <c r="F34" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G34" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H34" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="I34" s="54" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B35" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C35" t="s">
+        <v>821</v>
+      </c>
+      <c r="D35" t="s">
+        <v>825</v>
+      </c>
+      <c r="E35" t="s">
+        <v>731</v>
+      </c>
+      <c r="F35" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G35" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H35" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="I35" s="54" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B36" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C36" t="s">
+        <v>822</v>
+      </c>
+      <c r="D36" t="s">
+        <v>826</v>
+      </c>
+      <c r="E36" t="s">
+        <v>731</v>
+      </c>
+      <c r="F36" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G36" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H36" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="I36" s="54" t="s">
+        <v>814</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A20" xr:uid="{8D76983D-28D8-40FA-81DF-50E84AF004E2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A36">
       <formula1>"Input,Output,Calculated"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F20" xr:uid="{5A23AC18-18EC-4ADD-813B-C42B62155790}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B36">
+      <formula1>"General,PD,LGD,CCF,ELBE,LGDD,SL"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F36">
       <formula1>"Datetime,Categorical,Numeric"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B20" xr:uid="{0603A4C1-7DAA-44AA-8103-97FDFBDD8906}">
-      <formula1>"General,PD,LGD,CCF,ELBE,LGDD,SL"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -15862,6 +16468,146 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <jc981bd8ab5b47fd91abb7684c0f405b xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Brussels</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0086b60c-6752-48fa-8e91-a8805d8608ed</TermId>
+        </TermInfo>
+      </Terms>
+    </jc981bd8ab5b47fd91abb7684c0f405b>
+    <i14ea8bbd518495ea0e20ac1ad18c527 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Campaign Materials</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10e3cb14-f0bd-4a0a-bb1a-58c7e26fd5e4</TermId>
+        </TermInfo>
+      </Terms>
+    </i14ea8bbd518495ea0e20ac1ad18c527>
+    <b4187e12891e46deb4d240a4b28bdb90 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b4187e12891e46deb4d240a4b28bdb90>
+    <TaxCatchAll xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Value>13</Value>
+      <Value>12</Value>
+      <Value>11</Value>
+    </TaxCatchAll>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <e0e024ccac5240e69ae9c38a41bfa7a5 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e0e024ccac5240e69ae9c38a41bfa7a5>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <Classification_x0020_Status xmlns="35818088-e62d-4edf-bbb6-409430aef268" xsi:nil="true"/>
+    <k8128b1c45734e36a24fce652bc7ffb7 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Quantitative Services</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8ac922a9-ccce-4035-83d6-3ab1113bed22</TermId>
+        </TermInfo>
+      </Terms>
+    </k8128b1c45734e36a24fce652bc7ffb7>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+    <_dlc_DocId xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">3KSVPJYEA2AR-1011915566-26</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
+      <Url>https://sites.ey.com/sites/QAS_BELGIUM/_layouts/15/DocIdRedir.aspx?ID=3KSVPJYEA2AR-1011915566-26</Url>
+      <Description>3KSVPJYEA2AR-1011915566-26</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
+      <UserInfo>
+        <DisplayName>Diego De Plaen</DisplayName>
+        <AccountId>56</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Antonio Millan Puebla</DisplayName>
+        <AccountId>31</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sander Vandevenne</DisplayName>
+        <AccountId>54</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="EY Collaboration Document" ma:contentTypeID="0x010100826318CDA76982469C2C3CD2CD58474101010039A9718220E30744AB05D9570037D8A1" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0a3d079c8d19385a693d7ea59f238e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="50c908b1-f277-4340-90a9-4611d0b0f078" xmlns:ns4="35818088-e62d-4edf-bbb6-409430aef268" xmlns:ns5="40c6704c-f77c-4b8a-96a1-a10a2e12c42b" xmlns:ns6="96860b88-8044-411d-9267-72f1d28f5ec3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0684eb5fe437c3d422fbfa93671a941" ns1:_="" ns2:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16206,146 +16952,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <jc981bd8ab5b47fd91abb7684c0f405b xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Brussels</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0086b60c-6752-48fa-8e91-a8805d8608ed</TermId>
-        </TermInfo>
-      </Terms>
-    </jc981bd8ab5b47fd91abb7684c0f405b>
-    <i14ea8bbd518495ea0e20ac1ad18c527 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Campaign Materials</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10e3cb14-f0bd-4a0a-bb1a-58c7e26fd5e4</TermId>
-        </TermInfo>
-      </Terms>
-    </i14ea8bbd518495ea0e20ac1ad18c527>
-    <b4187e12891e46deb4d240a4b28bdb90 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b4187e12891e46deb4d240a4b28bdb90>
-    <TaxCatchAll xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Value>13</Value>
-      <Value>12</Value>
-      <Value>11</Value>
-    </TaxCatchAll>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <e0e024ccac5240e69ae9c38a41bfa7a5 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </e0e024ccac5240e69ae9c38a41bfa7a5>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <Classification_x0020_Status xmlns="35818088-e62d-4edf-bbb6-409430aef268" xsi:nil="true"/>
-    <k8128b1c45734e36a24fce652bc7ffb7 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Quantitative Services</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8ac922a9-ccce-4035-83d6-3ab1113bed22</TermId>
-        </TermInfo>
-      </Terms>
-    </k8128b1c45734e36a24fce652bc7ffb7>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-    <_dlc_DocId xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">3KSVPJYEA2AR-1011915566-26</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
-      <Url>https://sites.ey.com/sites/QAS_BELGIUM/_layouts/15/DocIdRedir.aspx?ID=3KSVPJYEA2AR-1011915566-26</Url>
-      <Description>3KSVPJYEA2AR-1011915566-26</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
-      <UserInfo>
-        <DisplayName>Diego De Plaen</DisplayName>
-        <AccountId>56</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Antonio Millan Puebla</DisplayName>
-        <AccountId>31</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sander Vandevenne</DisplayName>
-        <AccountId>54</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4AB6DE9-C584-4E87-8FF5-1A82C035629B}">
   <ds:schemaRefs>
@@ -16355,6 +16961,42 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65E10CC5-2433-4DC9-9A6B-251C7485D767}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D6130A-D52D-416E-88B9-F6885590E854}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A2966CE-FBFB-42D6-8AF5-4361359F35A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="50c908b1-f277-4340-90a9-4611d0b0f078"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="35818088-e62d-4edf-bbb6-409430aef268"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="96860b88-8044-411d-9267-72f1d28f5ec3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="40c6704c-f77c-4b8a-96a1-a10a2e12c42b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2D0B982-DBCA-4EED-A652-6CD257CDA216}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16374,40 +17016,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A2966CE-FBFB-42D6-8AF5-4361359F35A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="50c908b1-f277-4340-90a9-4611d0b0f078"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="35818088-e62d-4edf-bbb6-409430aef268"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="96860b88-8044-411d-9267-72f1d28f5ec3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="40c6704c-f77c-4b8a-96a1-a10a2e12c42b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D6130A-D52D-416E-88B9-F6885590E854}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65E10CC5-2433-4DC9-9A6B-251C7485D767}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
PD data model completed according to Brent's template
</commit_message>
<xml_diff>
--- a/IRB models/Data Model.xlsx
+++ b/IRB models/Data Model.xlsx
@@ -32,7 +32,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
-  <calcPr calcId="171027" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -442,93 +442,8 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Sander Vandevenne</author>
-  </authors>
-  <commentList>
-    <comment ref="C22" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sander Vandevenne:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Should be unique</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C24" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sander Vandevenne:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This should be unique: How to cope with Default_binary serving as an input to multiple other 'technical names'?
-Note that previously the idea was captured by the 'precedent(s)' and dependent(s)' columns.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C25" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sander Vandevenne:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-The grade and portfolio 'names' are duplicated information. In general, how to handle: 
-1. The same output needed to be reported at multiple instances (e.g. across parameter templates).
-2. Calculated or input 'technical' names that serve as input to multiple parameters </t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="888">
   <si>
     <t>LoanStatNew</t>
   </si>
@@ -3085,13 +3000,181 @@
     <t>Section 2.5.3: The original exposure at the beginning of the relevant observation period.</t>
   </si>
   <si>
-    <t>No explicit definition found</t>
-  </si>
-  <si>
     <t>PD_tests</t>
   </si>
   <si>
     <t>Jeffrey</t>
+  </si>
+  <si>
+    <t>Section 2.5 footnote 21</t>
+  </si>
+  <si>
+    <t>PD_AUC_val</t>
+  </si>
+  <si>
+    <t>PD_s_val</t>
+  </si>
+  <si>
+    <t>PD_AUC_dev</t>
+  </si>
+  <si>
+    <t>PD_AUC_S</t>
+  </si>
+  <si>
+    <t>PD_AUC_p</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 4.0      cell: D7</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 4.0      cell: E7</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 4.0      cell: F7</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 4.0      cell: G7</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 4.0      cell: H7</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>Section 3.1: AUC of the current period</t>
+  </si>
+  <si>
+    <t>Section 3.1: AUC of the development period</t>
+  </si>
+  <si>
+    <t>Section 3.1: AUC test statistic</t>
+  </si>
+  <si>
+    <t>Section 3.1: p-value of AUC test statistic</t>
+  </si>
+  <si>
+    <t>Section 2.5.5.1: Upper matrix weighted bandwidth</t>
+  </si>
+  <si>
+    <t>Section 2.5: Footnote 21 transformation</t>
+  </si>
+  <si>
+    <t>Section 3.1: Variance of the AUC of the current period</t>
+  </si>
+  <si>
+    <t>Section 2.5.5.1: Lower matrix weighted bandwidth</t>
+  </si>
+  <si>
+    <t>MWB</t>
+  </si>
+  <si>
+    <t>transition_matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section 2.5.5.1: Rating transition matrix </t>
+  </si>
+  <si>
+    <t>transition_matrix_freq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section 2.5.5.1: Relative rating transition matrix </t>
+  </si>
+  <si>
+    <t>Bin_PD</t>
+  </si>
+  <si>
+    <t>z_up</t>
+  </si>
+  <si>
+    <t>z_low</t>
+  </si>
+  <si>
+    <t>zUP_pval</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 5.1      cell: D7</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 5.1      cell: E7</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 5.2      cell: upper triangular z-values</t>
+  </si>
+  <si>
+    <t>zDOWN_pval</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 5.2      cell: upper triangular p-values</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 5.2      cell: lower triangular z-values</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 5.2      cell: lower triangular p-values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section 2.5.5.2: z-statistics transition </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section 2.5.5.2: probability-statistics transition </t>
+  </si>
+  <si>
+    <t>stability_migration_matrix</t>
+  </si>
+  <si>
+    <t>cr_pval</t>
+  </si>
+  <si>
+    <t>HI_curr_exp</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 4.0      cell: D18</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 4.0      cell: E18</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 4.0      cell: F18</t>
+  </si>
+  <si>
+    <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 4.0      cell: G18</t>
+  </si>
+  <si>
+    <t>Section 2.5.5.3: Herfindahl index at the beginning of the observation period</t>
+  </si>
+  <si>
+    <t>Section 2.5.5.3: Herfindahl index at the end of the observation period</t>
+  </si>
+  <si>
+    <t>Section 2.5.5.3: p-val of change in concentration</t>
+  </si>
+  <si>
+    <t>Section 2.5.5.3: Herfindahl index at the end of the observation period (exposure weighted)</t>
+  </si>
+  <si>
+    <t>Herfindahl</t>
+  </si>
+  <si>
+    <t>Section 2.5: Footnote 21</t>
+  </si>
+  <si>
+    <t>Section 2.5 Footnote 21</t>
   </si>
 </sst>
 </file>
@@ -4018,7 +4101,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4185,6 +4268,7 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="37" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4233,7 +4317,7 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="88">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4325,7 +4409,21 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -7439,74 +7537,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="93" t="s">
         <v>562</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="94"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="95"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="95"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="97"/>
+      <c r="A2" s="96"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="98"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="89" t="s">
         <v>563</v>
       </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="90"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="91"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>564</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="99" t="s">
         <v>565</v>
       </c>
-      <c r="C5" s="99"/>
-      <c r="D5" s="100"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="101"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>566</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="99" t="s">
         <v>567</v>
       </c>
-      <c r="C6" s="99"/>
-      <c r="D6" s="100"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="101"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>568</v>
       </c>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="102" t="s">
         <v>569</v>
       </c>
-      <c r="C7" s="102"/>
-      <c r="D7" s="103"/>
+      <c r="C7" s="103"/>
+      <c r="D7" s="104"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
         <v>570</v>
       </c>
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="102" t="s">
         <v>571</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="103"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="104"/>
     </row>
     <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="89" t="s">
         <v>572</v>
       </c>
-      <c r="B10" s="89"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="90"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="91"/>
     </row>
     <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
@@ -7566,12 +7664,12 @@
     </row>
     <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="91" t="s">
+      <c r="A17" s="92" t="s">
         <v>585</v>
       </c>
-      <c r="B17" s="91"/>
-      <c r="C17" s="91"/>
-      <c r="D17" s="91"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92"/>
     </row>
     <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -15359,12 +15457,12 @@
   </sheetData>
   <autoFilter ref="A1:P70"/>
   <conditionalFormatting sqref="A1:A9 A57:A70 A11:A55">
-    <cfRule type="containsBlanks" dxfId="1" priority="3">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(A10))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15399,12 +15497,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15454,144 +15552,146 @@
         <v>645</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>463</v>
+        <v>614</v>
       </c>
       <c r="C2" t="s">
-        <v>463</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>774</v>
-      </c>
-      <c r="E2" t="s">
+        <v>887</v>
+      </c>
+      <c r="E2" s="88" t="str">
+        <f>$E$62</f>
+        <v>create_data_set</v>
+      </c>
+      <c r="F2" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G2" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="H2" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="I2" s="83" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="83" t="s">
+        <v>645</v>
+      </c>
+      <c r="B3" s="83" t="s">
+        <v>365</v>
+      </c>
+      <c r="C3" s="88" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3" s="88" t="s">
+        <v>827</v>
+      </c>
+      <c r="E3" s="88" t="str">
+        <f>$E$62</f>
+        <v>create_data_set</v>
+      </c>
+      <c r="F3" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G3" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="H3" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="I3" s="83" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="83" t="s">
+        <v>645</v>
+      </c>
+      <c r="B4" s="83" t="s">
+        <v>614</v>
+      </c>
+      <c r="C4" s="88" t="s">
+        <v>392</v>
+      </c>
+      <c r="D4" s="88" t="s">
+        <v>777</v>
+      </c>
+      <c r="E4" s="88" t="s">
         <v>729</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F4" s="83" t="s">
         <v>647</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="G4" s="83" t="s">
         <v>795</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H4" s="83" t="s">
         <v>795</v>
       </c>
-      <c r="I2" s="54" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
-        <v>645</v>
-      </c>
-      <c r="B3" s="54" t="s">
-        <v>463</v>
-      </c>
-      <c r="C3" t="s">
-        <v>624</v>
-      </c>
-      <c r="D3" t="s">
-        <v>773</v>
-      </c>
-      <c r="E3" t="s">
-        <v>729</v>
-      </c>
-      <c r="F3" s="54" t="s">
-        <v>647</v>
-      </c>
-      <c r="G3" s="54" t="s">
-        <v>795</v>
-      </c>
-      <c r="H3" s="54" t="s">
-        <v>795</v>
-      </c>
-      <c r="I3" s="54" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="54" t="s">
-        <v>645</v>
-      </c>
-      <c r="B4" s="54" t="s">
-        <v>463</v>
-      </c>
-      <c r="C4" t="s">
-        <v>775</v>
-      </c>
-      <c r="D4" t="s">
-        <v>785</v>
-      </c>
-      <c r="E4" t="s">
-        <v>729</v>
-      </c>
-      <c r="F4" s="54" t="s">
-        <v>647</v>
-      </c>
-      <c r="G4" s="54" t="s">
-        <v>795</v>
-      </c>
-      <c r="H4" s="54" t="s">
-        <v>795</v>
-      </c>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="83" t="s">
         <v>795</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="54" t="s">
-        <v>645</v>
+        <v>659</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C5" t="s">
-        <v>776</v>
-      </c>
-      <c r="D5" t="s">
-        <v>786</v>
+        <v>817</v>
+      </c>
+      <c r="D5" s="88" t="s">
+        <v>828</v>
       </c>
       <c r="E5" t="s">
-        <v>729</v>
-      </c>
-      <c r="F5" s="54" t="s">
+        <v>731</v>
+      </c>
+      <c r="F5" s="83" t="s">
         <v>647</v>
       </c>
       <c r="G5" s="54" t="s">
-        <v>795</v>
-      </c>
-      <c r="H5" s="54" t="s">
-        <v>795</v>
-      </c>
-      <c r="I5" s="54" t="s">
-        <v>795</v>
+        <v>730</v>
+      </c>
+      <c r="H5" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I5" s="83" t="s">
+        <v>835</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="54" t="s">
-        <v>645</v>
+        <v>659</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C6" t="s">
-        <v>392</v>
-      </c>
-      <c r="D6" t="s">
-        <v>777</v>
+        <v>818</v>
+      </c>
+      <c r="D6" s="88" t="s">
+        <v>829</v>
       </c>
       <c r="E6" t="s">
-        <v>729</v>
-      </c>
-      <c r="F6" s="54" t="s">
+        <v>731</v>
+      </c>
+      <c r="F6" s="83" t="s">
         <v>647</v>
       </c>
       <c r="G6" s="54" t="s">
-        <v>795</v>
-      </c>
-      <c r="H6" s="54" t="s">
-        <v>795</v>
-      </c>
-      <c r="I6" s="54" t="s">
-        <v>795</v>
+        <v>730</v>
+      </c>
+      <c r="H6" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I6" s="83" t="s">
+        <v>835</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -15599,28 +15699,28 @@
         <v>659</v>
       </c>
       <c r="B7" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C7" t="s">
-        <v>725</v>
-      </c>
-      <c r="D7" t="s">
-        <v>787</v>
+        <v>819</v>
+      </c>
+      <c r="D7" s="88" t="s">
+        <v>830</v>
       </c>
       <c r="E7" t="s">
         <v>731</v>
       </c>
-      <c r="F7" s="54" t="s">
+      <c r="F7" s="83" t="s">
         <v>647</v>
       </c>
       <c r="G7" s="54" t="s">
         <v>730</v>
       </c>
-      <c r="H7" s="54" t="s">
-        <v>810</v>
-      </c>
-      <c r="I7" s="54" t="s">
-        <v>811</v>
+      <c r="H7" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I7" s="83" t="s">
+        <v>835</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -15628,28 +15728,28 @@
         <v>659</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C8" t="s">
-        <v>778</v>
-      </c>
-      <c r="D8" t="s">
-        <v>788</v>
+        <v>820</v>
+      </c>
+      <c r="D8" s="88" t="s">
+        <v>831</v>
       </c>
       <c r="E8" t="s">
         <v>731</v>
       </c>
-      <c r="F8" s="54" t="s">
+      <c r="F8" s="83" t="s">
         <v>647</v>
       </c>
       <c r="G8" s="54" t="s">
         <v>730</v>
       </c>
-      <c r="H8" s="54" t="s">
-        <v>810</v>
-      </c>
-      <c r="I8" s="54" t="s">
-        <v>812</v>
+      <c r="H8" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I8" s="83" t="s">
+        <v>835</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -15657,28 +15757,28 @@
         <v>659</v>
       </c>
       <c r="B9" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C9" t="s">
-        <v>724</v>
-      </c>
-      <c r="D9" t="s">
-        <v>790</v>
+        <v>821</v>
+      </c>
+      <c r="D9" s="88" t="s">
+        <v>832</v>
       </c>
       <c r="E9" t="s">
         <v>731</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="83" t="s">
         <v>647</v>
       </c>
       <c r="G9" s="54" t="s">
         <v>730</v>
       </c>
-      <c r="H9" s="54" t="s">
-        <v>810</v>
-      </c>
-      <c r="I9" s="54" t="s">
-        <v>811</v>
+      <c r="H9" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I9" s="83" t="s">
+        <v>835</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -15686,42 +15786,42 @@
         <v>659</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C10" t="s">
-        <v>779</v>
-      </c>
-      <c r="D10" t="s">
-        <v>789</v>
+        <v>822</v>
+      </c>
+      <c r="D10" s="88" t="s">
+        <v>833</v>
       </c>
       <c r="E10" t="s">
         <v>731</v>
       </c>
-      <c r="F10" s="54" t="s">
+      <c r="F10" s="83" t="s">
         <v>647</v>
       </c>
       <c r="G10" s="54" t="s">
         <v>730</v>
       </c>
-      <c r="H10" s="54" t="s">
-        <v>810</v>
-      </c>
-      <c r="I10" s="54" t="s">
-        <v>812</v>
+      <c r="H10" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I10" s="83" t="s">
+        <v>835</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="54" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="B11" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C11" t="s">
-        <v>780</v>
+        <v>817</v>
       </c>
       <c r="D11" t="s">
-        <v>791</v>
+        <v>815</v>
       </c>
       <c r="E11" t="s">
         <v>731</v>
@@ -15730,27 +15830,27 @@
         <v>647</v>
       </c>
       <c r="G11" s="54" t="s">
-        <v>730</v>
+        <v>798</v>
       </c>
       <c r="H11" s="54" t="s">
-        <v>809</v>
-      </c>
-      <c r="I11" t="s">
-        <v>723</v>
+        <v>798</v>
+      </c>
+      <c r="I11" s="54" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="54" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="B12" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C12" t="s">
-        <v>781</v>
+        <v>818</v>
       </c>
       <c r="D12" t="s">
-        <v>792</v>
+        <v>816</v>
       </c>
       <c r="E12" t="s">
         <v>731</v>
@@ -15759,27 +15859,27 @@
         <v>647</v>
       </c>
       <c r="G12" s="54" t="s">
-        <v>730</v>
+        <v>798</v>
       </c>
       <c r="H12" s="54" t="s">
-        <v>809</v>
-      </c>
-      <c r="I12" t="s">
-        <v>723</v>
+        <v>798</v>
+      </c>
+      <c r="I12" s="54" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="54" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="B13" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C13" t="s">
-        <v>803</v>
+        <v>819</v>
       </c>
       <c r="D13" t="s">
-        <v>804</v>
+        <v>823</v>
       </c>
       <c r="E13" t="s">
         <v>731</v>
@@ -15788,27 +15888,27 @@
         <v>647</v>
       </c>
       <c r="G13" s="54" t="s">
-        <v>730</v>
+        <v>798</v>
       </c>
       <c r="H13" s="54" t="s">
-        <v>809</v>
-      </c>
-      <c r="I13" t="s">
-        <v>723</v>
+        <v>798</v>
+      </c>
+      <c r="I13" s="54" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="54" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="B14" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C14" t="s">
-        <v>782</v>
+        <v>820</v>
       </c>
       <c r="D14" t="s">
-        <v>802</v>
+        <v>824</v>
       </c>
       <c r="E14" t="s">
         <v>731</v>
@@ -15817,27 +15917,27 @@
         <v>647</v>
       </c>
       <c r="G14" s="54" t="s">
-        <v>730</v>
+        <v>798</v>
       </c>
       <c r="H14" s="54" t="s">
-        <v>809</v>
-      </c>
-      <c r="I14" t="s">
-        <v>723</v>
+        <v>798</v>
+      </c>
+      <c r="I14" s="54" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="54" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="B15" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C15" t="s">
-        <v>783</v>
+        <v>821</v>
       </c>
       <c r="D15" t="s">
-        <v>793</v>
+        <v>825</v>
       </c>
       <c r="E15" t="s">
         <v>731</v>
@@ -15846,13 +15946,13 @@
         <v>647</v>
       </c>
       <c r="G15" s="54" t="s">
-        <v>730</v>
+        <v>798</v>
       </c>
       <c r="H15" s="54" t="s">
-        <v>809</v>
-      </c>
-      <c r="I15" t="s">
-        <v>723</v>
+        <v>798</v>
+      </c>
+      <c r="I15" s="54" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -15860,13 +15960,13 @@
         <v>646</v>
       </c>
       <c r="B16" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C16" t="s">
-        <v>780</v>
-      </c>
-      <c r="D16" s="54" t="s">
-        <v>797</v>
+        <v>822</v>
+      </c>
+      <c r="D16" t="s">
+        <v>826</v>
       </c>
       <c r="E16" t="s">
         <v>731</v>
@@ -15877,83 +15977,84 @@
       <c r="G16" s="54" t="s">
         <v>798</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="54" t="s">
         <v>798</v>
       </c>
-      <c r="I16" t="s">
-        <v>813</v>
+      <c r="I16" s="54" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="B17" s="54" t="s">
-        <v>463</v>
-      </c>
-      <c r="C17" t="s">
-        <v>781</v>
-      </c>
-      <c r="D17" s="54" t="s">
-        <v>799</v>
-      </c>
-      <c r="E17" t="s">
-        <v>731</v>
-      </c>
-      <c r="F17" s="54" t="s">
+      <c r="A17" s="83" t="s">
+        <v>645</v>
+      </c>
+      <c r="B17" s="83" t="s">
+        <v>614</v>
+      </c>
+      <c r="C17" s="88" t="s">
+        <v>732</v>
+      </c>
+      <c r="D17" t="s">
+        <v>853</v>
+      </c>
+      <c r="E17" s="88" t="str">
+        <f>$E$62</f>
+        <v>create_data_set</v>
+      </c>
+      <c r="F17" s="83" t="s">
         <v>647</v>
       </c>
-      <c r="G17" s="54" t="s">
-        <v>798</v>
-      </c>
-      <c r="H17" t="s">
-        <v>798</v>
-      </c>
-      <c r="I17" t="s">
-        <v>813</v>
+      <c r="G17" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="H17" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="I17" s="83" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="B18" s="54" t="s">
-        <v>463</v>
-      </c>
-      <c r="C18" t="s">
-        <v>803</v>
-      </c>
-      <c r="D18" s="54" t="s">
-        <v>800</v>
+      <c r="A18" s="83" t="s">
+        <v>645</v>
+      </c>
+      <c r="B18" s="83" t="s">
+        <v>614</v>
+      </c>
+      <c r="C18" s="88" t="s">
+        <v>392</v>
+      </c>
+      <c r="D18" t="s">
+        <v>777</v>
       </c>
       <c r="E18" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F18" s="54" t="s">
         <v>647</v>
       </c>
       <c r="G18" s="54" t="s">
-        <v>798</v>
-      </c>
-      <c r="H18" t="s">
-        <v>798</v>
-      </c>
-      <c r="I18" t="s">
-        <v>813</v>
+        <v>795</v>
+      </c>
+      <c r="H18" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="I18" s="54" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="54" t="s">
-        <v>646</v>
+        <v>659</v>
       </c>
       <c r="B19" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C19" t="s">
-        <v>782</v>
-      </c>
-      <c r="D19" s="54" t="s">
-        <v>801</v>
+        <v>837</v>
+      </c>
+      <c r="D19" t="s">
+        <v>848</v>
       </c>
       <c r="E19" t="s">
         <v>731</v>
@@ -15962,27 +16063,27 @@
         <v>647</v>
       </c>
       <c r="G19" s="54" t="s">
-        <v>798</v>
-      </c>
-      <c r="H19" t="s">
-        <v>798</v>
-      </c>
-      <c r="I19" t="s">
-        <v>813</v>
+        <v>730</v>
+      </c>
+      <c r="H19" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I19" s="83" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="54" t="s">
-        <v>646</v>
+        <v>659</v>
       </c>
       <c r="B20" s="54" t="s">
-        <v>463</v>
+        <v>365</v>
       </c>
       <c r="C20" t="s">
-        <v>783</v>
-      </c>
-      <c r="D20" s="54" t="s">
-        <v>805</v>
+        <v>839</v>
+      </c>
+      <c r="D20" t="s">
+        <v>849</v>
       </c>
       <c r="E20" t="s">
         <v>731</v>
@@ -15991,326 +16092,348 @@
         <v>647</v>
       </c>
       <c r="G20" s="54" t="s">
-        <v>798</v>
-      </c>
-      <c r="H20" t="s">
-        <v>798</v>
-      </c>
-      <c r="I20" t="s">
-        <v>813</v>
+        <v>730</v>
+      </c>
+      <c r="H20" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I20" s="83" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
-      <c r="B21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
+      <c r="A21" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B21" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C21" t="s">
+        <v>838</v>
+      </c>
+      <c r="D21" t="s">
+        <v>854</v>
+      </c>
+      <c r="E21" t="s">
+        <v>731</v>
+      </c>
+      <c r="F21" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G21" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H21" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I21" s="83" t="s">
+        <v>847</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="54" t="s">
-        <v>645</v>
+        <v>659</v>
       </c>
       <c r="B22" s="54" t="s">
         <v>365</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="83" t="s">
+        <v>840</v>
+      </c>
+      <c r="D22" t="s">
+        <v>850</v>
+      </c>
+      <c r="E22" t="s">
+        <v>731</v>
+      </c>
+      <c r="F22" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G22" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H22" s="83" t="s">
         <v>834</v>
       </c>
-      <c r="E22" s="104" t="str">
-        <f>$E$2</f>
-        <v>create_data_set</v>
-      </c>
-      <c r="F22" s="83" t="s">
+      <c r="I22" s="83" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B23" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C23" t="s">
+        <v>841</v>
+      </c>
+      <c r="D23" t="s">
+        <v>851</v>
+      </c>
+      <c r="E23" t="s">
+        <v>731</v>
+      </c>
+      <c r="F23" s="54" t="s">
         <v>647</v>
       </c>
-      <c r="G22" s="83" t="s">
-        <v>795</v>
-      </c>
-      <c r="H22" s="83" t="s">
-        <v>795</v>
-      </c>
-      <c r="I22" s="83" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="83" t="s">
-        <v>645</v>
-      </c>
-      <c r="B23" s="83" t="s">
+      <c r="G23" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H23" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I23" s="83" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B24" s="54" t="s">
         <v>365</v>
       </c>
-      <c r="C23" s="104" t="s">
-        <v>365</v>
-      </c>
-      <c r="D23" s="104" t="s">
-        <v>827</v>
-      </c>
-      <c r="E23" s="104" t="str">
-        <f>$E$2</f>
-        <v>create_data_set</v>
-      </c>
-      <c r="F23" s="83" t="s">
+      <c r="C24" t="s">
+        <v>837</v>
+      </c>
+      <c r="D24" t="s">
+        <v>842</v>
+      </c>
+      <c r="E24" t="s">
+        <v>731</v>
+      </c>
+      <c r="F24" s="54" t="s">
         <v>647</v>
       </c>
-      <c r="G23" s="83" t="s">
-        <v>795</v>
-      </c>
-      <c r="H23" s="83" t="s">
-        <v>795</v>
-      </c>
-      <c r="I23" s="83" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="83" t="s">
-        <v>645</v>
-      </c>
-      <c r="B24" s="83" t="s">
-        <v>365</v>
-      </c>
-      <c r="C24" s="104" t="s">
-        <v>392</v>
-      </c>
-      <c r="D24" s="104" t="s">
-        <v>777</v>
-      </c>
-      <c r="E24" s="104" t="s">
-        <v>729</v>
-      </c>
-      <c r="F24" s="83" t="s">
-        <v>647</v>
-      </c>
-      <c r="G24" s="83" t="s">
-        <v>795</v>
-      </c>
-      <c r="H24" s="83" t="s">
-        <v>795</v>
-      </c>
-      <c r="I24" s="83" t="s">
-        <v>795</v>
+      <c r="G24" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H24" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="I24" s="54" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="54" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="B25" s="54" t="s">
         <v>365</v>
       </c>
       <c r="C25" t="s">
-        <v>817</v>
-      </c>
-      <c r="D25" s="104" t="s">
-        <v>828</v>
+        <v>839</v>
+      </c>
+      <c r="D25" t="s">
+        <v>843</v>
       </c>
       <c r="E25" t="s">
         <v>731</v>
       </c>
-      <c r="F25" s="83" t="s">
+      <c r="F25" s="54" t="s">
         <v>647</v>
       </c>
       <c r="G25" s="54" t="s">
-        <v>730</v>
-      </c>
-      <c r="H25" s="83" t="s">
-        <v>835</v>
-      </c>
-      <c r="I25" s="83" t="s">
-        <v>836</v>
+        <v>798</v>
+      </c>
+      <c r="H25" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="I25" s="54" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="54" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="B26" s="54" t="s">
         <v>365</v>
       </c>
       <c r="C26" t="s">
-        <v>818</v>
-      </c>
-      <c r="D26" s="104" t="s">
-        <v>829</v>
+        <v>838</v>
+      </c>
+      <c r="D26" t="s">
+        <v>844</v>
       </c>
       <c r="E26" t="s">
         <v>731</v>
       </c>
-      <c r="F26" s="83" t="s">
+      <c r="F26" s="54" t="s">
         <v>647</v>
       </c>
       <c r="G26" s="54" t="s">
-        <v>730</v>
-      </c>
-      <c r="H26" s="83" t="s">
-        <v>835</v>
-      </c>
-      <c r="I26" s="83" t="s">
-        <v>836</v>
+        <v>798</v>
+      </c>
+      <c r="H26" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="I26" s="54" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="54" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="B27" s="54" t="s">
         <v>365</v>
       </c>
       <c r="C27" t="s">
-        <v>819</v>
-      </c>
-      <c r="D27" s="104" t="s">
-        <v>830</v>
+        <v>840</v>
+      </c>
+      <c r="D27" t="s">
+        <v>845</v>
       </c>
       <c r="E27" t="s">
         <v>731</v>
       </c>
-      <c r="F27" s="83" t="s">
+      <c r="F27" s="54" t="s">
         <v>647</v>
       </c>
       <c r="G27" s="54" t="s">
-        <v>730</v>
-      </c>
-      <c r="H27" s="83" t="s">
-        <v>835</v>
-      </c>
-      <c r="I27" s="83" t="s">
-        <v>836</v>
+        <v>798</v>
+      </c>
+      <c r="H27" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="I27" s="54" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="54" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="B28" s="54" t="s">
         <v>365</v>
       </c>
       <c r="C28" t="s">
-        <v>820</v>
-      </c>
-      <c r="D28" s="104" t="s">
-        <v>831</v>
+        <v>841</v>
+      </c>
+      <c r="D28" t="s">
+        <v>846</v>
       </c>
       <c r="E28" t="s">
         <v>731</v>
       </c>
-      <c r="F28" s="83" t="s">
+      <c r="F28" s="54" t="s">
         <v>647</v>
       </c>
       <c r="G28" s="54" t="s">
-        <v>730</v>
-      </c>
-      <c r="H28" s="83" t="s">
-        <v>835</v>
-      </c>
-      <c r="I28" s="83" t="s">
-        <v>836</v>
+        <v>798</v>
+      </c>
+      <c r="H28" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="I28" s="54" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="54" t="s">
-        <v>659</v>
+        <v>645</v>
       </c>
       <c r="B29" s="54" t="s">
         <v>365</v>
       </c>
       <c r="C29" t="s">
-        <v>821</v>
-      </c>
-      <c r="D29" s="104" t="s">
-        <v>832</v>
-      </c>
-      <c r="E29" t="s">
-        <v>731</v>
+        <v>861</v>
+      </c>
+      <c r="D29" t="s">
+        <v>887</v>
+      </c>
+      <c r="E29" s="88" t="str">
+        <f>$E$62</f>
+        <v>create_data_set</v>
       </c>
       <c r="F29" s="83" t="s">
         <v>647</v>
       </c>
-      <c r="G29" s="54" t="s">
-        <v>730</v>
+      <c r="G29" s="83" t="s">
+        <v>795</v>
       </c>
       <c r="H29" s="83" t="s">
-        <v>835</v>
+        <v>795</v>
       </c>
       <c r="I29" s="83" t="s">
-        <v>836</v>
+        <v>795</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="54" t="s">
-        <v>659</v>
+        <v>645</v>
       </c>
       <c r="B30" s="54" t="s">
-        <v>365</v>
-      </c>
-      <c r="C30" t="s">
-        <v>822</v>
-      </c>
-      <c r="D30" s="104" t="s">
-        <v>833</v>
-      </c>
-      <c r="E30" t="s">
-        <v>731</v>
+        <v>614</v>
+      </c>
+      <c r="C30" s="88" t="s">
+        <v>732</v>
+      </c>
+      <c r="D30" t="s">
+        <v>853</v>
+      </c>
+      <c r="E30" s="88" t="str">
+        <f>$E$62</f>
+        <v>create_data_set</v>
       </c>
       <c r="F30" s="83" t="s">
         <v>647</v>
       </c>
-      <c r="G30" s="54" t="s">
-        <v>730</v>
+      <c r="G30" s="83" t="s">
+        <v>795</v>
       </c>
       <c r="H30" s="83" t="s">
-        <v>835</v>
+        <v>795</v>
       </c>
       <c r="I30" s="83" t="s">
-        <v>836</v>
+        <v>795</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="54" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B31" s="54" t="s">
-        <v>365</v>
-      </c>
-      <c r="C31" t="s">
-        <v>817</v>
+        <v>614</v>
+      </c>
+      <c r="C31" s="88" t="s">
+        <v>392</v>
       </c>
       <c r="D31" t="s">
-        <v>815</v>
+        <v>777</v>
       </c>
       <c r="E31" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F31" s="54" t="s">
         <v>647</v>
       </c>
       <c r="G31" s="54" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="H31" s="54" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="I31" s="54" t="s">
-        <v>814</v>
+        <v>795</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="54" t="s">
-        <v>646</v>
+        <v>659</v>
       </c>
       <c r="B32" s="54" t="s">
         <v>365</v>
       </c>
       <c r="C32" t="s">
-        <v>818</v>
+        <v>857</v>
       </c>
       <c r="D32" t="s">
-        <v>816</v>
+        <v>858</v>
       </c>
       <c r="E32" t="s">
         <v>731</v>
@@ -16319,27 +16442,27 @@
         <v>647</v>
       </c>
       <c r="G32" s="54" t="s">
-        <v>798</v>
+        <v>730</v>
       </c>
       <c r="H32" s="54" t="s">
-        <v>798</v>
+        <v>810</v>
       </c>
       <c r="I32" s="54" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="54" t="s">
-        <v>646</v>
+        <v>659</v>
       </c>
       <c r="B33" s="54" t="s">
         <v>365</v>
       </c>
       <c r="C33" t="s">
-        <v>819</v>
+        <v>859</v>
       </c>
       <c r="D33" t="s">
-        <v>823</v>
+        <v>860</v>
       </c>
       <c r="E33" t="s">
         <v>731</v>
@@ -16348,27 +16471,27 @@
         <v>647</v>
       </c>
       <c r="G33" s="54" t="s">
-        <v>798</v>
+        <v>730</v>
       </c>
       <c r="H33" s="54" t="s">
-        <v>798</v>
+        <v>810</v>
       </c>
       <c r="I33" s="54" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="54" t="s">
-        <v>646</v>
+        <v>659</v>
       </c>
       <c r="B34" s="54" t="s">
         <v>365</v>
       </c>
       <c r="C34" t="s">
-        <v>820</v>
+        <v>455</v>
       </c>
       <c r="D34" t="s">
-        <v>824</v>
+        <v>852</v>
       </c>
       <c r="E34" t="s">
         <v>731</v>
@@ -16377,27 +16500,27 @@
         <v>647</v>
       </c>
       <c r="G34" s="54" t="s">
-        <v>798</v>
-      </c>
-      <c r="H34" s="54" t="s">
-        <v>798</v>
-      </c>
-      <c r="I34" s="54" t="s">
-        <v>814</v>
+        <v>730</v>
+      </c>
+      <c r="H34" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I34" s="83" t="s">
+        <v>856</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="54" t="s">
-        <v>646</v>
+        <v>659</v>
       </c>
       <c r="B35" s="54" t="s">
         <v>365</v>
       </c>
       <c r="C35" t="s">
-        <v>821</v>
+        <v>453</v>
       </c>
       <c r="D35" t="s">
-        <v>825</v>
+        <v>855</v>
       </c>
       <c r="E35" t="s">
         <v>731</v>
@@ -16406,13 +16529,13 @@
         <v>647</v>
       </c>
       <c r="G35" s="54" t="s">
-        <v>798</v>
-      </c>
-      <c r="H35" s="54" t="s">
-        <v>798</v>
-      </c>
-      <c r="I35" s="54" t="s">
-        <v>814</v>
+        <v>730</v>
+      </c>
+      <c r="H35" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I35" s="83" t="s">
+        <v>856</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -16423,10 +16546,10 @@
         <v>365</v>
       </c>
       <c r="C36" t="s">
-        <v>822</v>
+        <v>455</v>
       </c>
       <c r="D36" t="s">
-        <v>826</v>
+        <v>865</v>
       </c>
       <c r="E36" t="s">
         <v>731</v>
@@ -16437,37 +16560,1290 @@
       <c r="G36" s="54" t="s">
         <v>798</v>
       </c>
-      <c r="H36" s="54" t="s">
+      <c r="H36" s="83" t="s">
         <v>798</v>
       </c>
-      <c r="I36" s="54" t="s">
+      <c r="I36" s="83" t="s">
         <v>814</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B37" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C37" t="s">
+        <v>453</v>
+      </c>
+      <c r="D37" t="s">
+        <v>866</v>
+      </c>
+      <c r="E37" t="s">
+        <v>731</v>
+      </c>
+      <c r="F37" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G37" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H37" s="83" t="s">
+        <v>798</v>
+      </c>
+      <c r="I37" s="83" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B38" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C38" t="s">
+        <v>861</v>
+      </c>
+      <c r="D38" t="s">
+        <v>836</v>
+      </c>
+      <c r="E38" s="88" t="str">
+        <f>$E$62</f>
+        <v>create_data_set</v>
+      </c>
+      <c r="F38" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G38" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="H38" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="I38" s="83" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B39" s="54" t="s">
+        <v>614</v>
+      </c>
+      <c r="C39" s="88" t="s">
+        <v>732</v>
+      </c>
+      <c r="D39" t="s">
+        <v>853</v>
+      </c>
+      <c r="E39" s="88" t="str">
+        <f>$E$62</f>
+        <v>create_data_set</v>
+      </c>
+      <c r="F39" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G39" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="H39" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="I39" s="83" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B40" s="54" t="s">
+        <v>614</v>
+      </c>
+      <c r="C40" s="88" t="s">
+        <v>392</v>
+      </c>
+      <c r="D40" t="s">
+        <v>777</v>
+      </c>
+      <c r="E40" t="s">
+        <v>729</v>
+      </c>
+      <c r="F40" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G40" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="H40" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="I40" s="54" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B41" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C41" t="s">
+        <v>857</v>
+      </c>
+      <c r="D41" t="s">
+        <v>858</v>
+      </c>
+      <c r="E41" t="s">
+        <v>731</v>
+      </c>
+      <c r="F41" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G41" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H41" s="54" t="s">
+        <v>810</v>
+      </c>
+      <c r="I41" s="54" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B42" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C42" t="s">
+        <v>859</v>
+      </c>
+      <c r="D42" t="s">
+        <v>860</v>
+      </c>
+      <c r="E42" t="s">
+        <v>731</v>
+      </c>
+      <c r="F42" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G42" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H42" s="54" t="s">
+        <v>810</v>
+      </c>
+      <c r="I42" s="54" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B43" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C43" t="s">
+        <v>862</v>
+      </c>
+      <c r="D43" t="s">
+        <v>872</v>
+      </c>
+      <c r="E43" t="s">
+        <v>731</v>
+      </c>
+      <c r="F43" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G43" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H43" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I43" s="83" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B44" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C44" t="s">
+        <v>863</v>
+      </c>
+      <c r="D44" t="s">
+        <v>872</v>
+      </c>
+      <c r="E44" t="s">
+        <v>731</v>
+      </c>
+      <c r="F44" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G44" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H44" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I44" s="83" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B45" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C45" t="s">
+        <v>864</v>
+      </c>
+      <c r="D45" t="s">
+        <v>873</v>
+      </c>
+      <c r="E45" t="s">
+        <v>731</v>
+      </c>
+      <c r="F45" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G45" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H45" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I45" s="83" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B46" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C46" t="s">
+        <v>868</v>
+      </c>
+      <c r="D46" t="s">
+        <v>873</v>
+      </c>
+      <c r="E46" t="s">
+        <v>731</v>
+      </c>
+      <c r="F46" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G46" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H46" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I46" s="83" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B47" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C47" t="s">
+        <v>862</v>
+      </c>
+      <c r="D47" t="s">
+        <v>867</v>
+      </c>
+      <c r="E47" t="s">
+        <v>731</v>
+      </c>
+      <c r="F47" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G47" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H47" s="83" t="s">
+        <v>798</v>
+      </c>
+      <c r="I47" s="83" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B48" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C48" t="s">
+        <v>863</v>
+      </c>
+      <c r="D48" t="s">
+        <v>870</v>
+      </c>
+      <c r="E48" t="s">
+        <v>731</v>
+      </c>
+      <c r="F48" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G48" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H48" s="83" t="s">
+        <v>798</v>
+      </c>
+      <c r="I48" s="83" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B49" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C49" t="s">
+        <v>864</v>
+      </c>
+      <c r="D49" t="s">
+        <v>869</v>
+      </c>
+      <c r="E49" t="s">
+        <v>731</v>
+      </c>
+      <c r="F49" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G49" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H49" s="83" t="s">
+        <v>798</v>
+      </c>
+      <c r="I49" s="83" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B50" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C50" t="s">
+        <v>868</v>
+      </c>
+      <c r="D50" t="s">
+        <v>871</v>
+      </c>
+      <c r="E50" t="s">
+        <v>731</v>
+      </c>
+      <c r="F50" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G50" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H50" s="83" t="s">
+        <v>798</v>
+      </c>
+      <c r="I50" s="83" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B51" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C51" t="s">
+        <v>861</v>
+      </c>
+      <c r="D51" t="s">
+        <v>887</v>
+      </c>
+      <c r="E51" s="88" t="str">
+        <f>$E$62</f>
+        <v>create_data_set</v>
+      </c>
+      <c r="F51" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G51" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="H51" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="I51" s="83" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B52" s="54" t="s">
+        <v>614</v>
+      </c>
+      <c r="C52" s="88" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" t="s">
+        <v>886</v>
+      </c>
+      <c r="E52" s="88" t="str">
+        <f>$E$62</f>
+        <v>create_data_set</v>
+      </c>
+      <c r="F52" s="83" t="s">
+        <v>647</v>
+      </c>
+      <c r="G52" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="H52" s="83" t="s">
+        <v>795</v>
+      </c>
+      <c r="I52" s="83" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B53" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C53" t="s">
+        <v>671</v>
+      </c>
+      <c r="D53" t="s">
+        <v>881</v>
+      </c>
+      <c r="E53" t="s">
+        <v>731</v>
+      </c>
+      <c r="F53" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G53" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H53" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I53" s="83" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B54" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C54" t="s">
+        <v>672</v>
+      </c>
+      <c r="D54" t="s">
+        <v>882</v>
+      </c>
+      <c r="E54" t="s">
+        <v>731</v>
+      </c>
+      <c r="F54" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G54" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H54" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I54" s="83" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B55" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C55" t="s">
+        <v>875</v>
+      </c>
+      <c r="D55" t="s">
+        <v>883</v>
+      </c>
+      <c r="E55" t="s">
+        <v>731</v>
+      </c>
+      <c r="F55" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G55" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H55" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I55" s="83" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B56" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C56" s="105" t="s">
+        <v>876</v>
+      </c>
+      <c r="D56" t="s">
+        <v>884</v>
+      </c>
+      <c r="E56" t="s">
+        <v>731</v>
+      </c>
+      <c r="F56" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G56" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H56" s="83" t="s">
+        <v>834</v>
+      </c>
+      <c r="I56" s="83" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B57" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C57" t="s">
+        <v>671</v>
+      </c>
+      <c r="D57" t="s">
+        <v>877</v>
+      </c>
+      <c r="E57" t="s">
+        <v>731</v>
+      </c>
+      <c r="F57" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G57" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H57" s="83" t="s">
+        <v>798</v>
+      </c>
+      <c r="I57" s="83" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B58" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C58" t="s">
+        <v>672</v>
+      </c>
+      <c r="D58" t="s">
+        <v>878</v>
+      </c>
+      <c r="E58" t="s">
+        <v>731</v>
+      </c>
+      <c r="F58" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G58" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H58" s="83" t="s">
+        <v>798</v>
+      </c>
+      <c r="I58" s="83" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B59" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C59" t="s">
+        <v>875</v>
+      </c>
+      <c r="D59" t="s">
+        <v>879</v>
+      </c>
+      <c r="E59" t="s">
+        <v>731</v>
+      </c>
+      <c r="F59" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G59" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H59" s="83" t="s">
+        <v>798</v>
+      </c>
+      <c r="I59" s="83" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B60" s="54" t="s">
+        <v>365</v>
+      </c>
+      <c r="C60" s="105" t="s">
+        <v>876</v>
+      </c>
+      <c r="D60" t="s">
+        <v>880</v>
+      </c>
+      <c r="E60" t="s">
+        <v>731</v>
+      </c>
+      <c r="F60" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G60" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H60" s="83" t="s">
+        <v>798</v>
+      </c>
+      <c r="I60" s="83" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="54"/>
+      <c r="B61" s="54"/>
+      <c r="F61" s="54"/>
+      <c r="G61" s="54"/>
+      <c r="H61" s="83"/>
+      <c r="I61" s="83"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B62" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C62" t="s">
+        <v>463</v>
+      </c>
+      <c r="D62" t="s">
+        <v>774</v>
+      </c>
+      <c r="E62" t="s">
+        <v>729</v>
+      </c>
+      <c r="F62" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G62" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="H62" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="I62" s="54" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B63" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C63" t="s">
+        <v>624</v>
+      </c>
+      <c r="D63" t="s">
+        <v>773</v>
+      </c>
+      <c r="E63" t="s">
+        <v>729</v>
+      </c>
+      <c r="F63" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G63" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="H63" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="I63" s="54" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B64" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C64" t="s">
+        <v>775</v>
+      </c>
+      <c r="D64" t="s">
+        <v>785</v>
+      </c>
+      <c r="E64" t="s">
+        <v>729</v>
+      </c>
+      <c r="F64" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G64" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="H64" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="I64" s="54" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B65" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C65" t="s">
+        <v>776</v>
+      </c>
+      <c r="D65" t="s">
+        <v>786</v>
+      </c>
+      <c r="E65" t="s">
+        <v>729</v>
+      </c>
+      <c r="F65" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G65" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="H65" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="I65" s="54" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="B66" s="54" t="s">
+        <v>614</v>
+      </c>
+      <c r="C66" t="s">
+        <v>392</v>
+      </c>
+      <c r="D66" t="s">
+        <v>777</v>
+      </c>
+      <c r="E66" t="s">
+        <v>729</v>
+      </c>
+      <c r="F66" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G66" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="H66" s="54" t="s">
+        <v>795</v>
+      </c>
+      <c r="I66" s="54" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B67" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C67" t="s">
+        <v>725</v>
+      </c>
+      <c r="D67" t="s">
+        <v>787</v>
+      </c>
+      <c r="E67" t="s">
+        <v>731</v>
+      </c>
+      <c r="F67" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G67" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H67" s="54" t="s">
+        <v>810</v>
+      </c>
+      <c r="I67" s="54" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B68" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C68" t="s">
+        <v>778</v>
+      </c>
+      <c r="D68" t="s">
+        <v>788</v>
+      </c>
+      <c r="E68" t="s">
+        <v>731</v>
+      </c>
+      <c r="F68" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G68" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H68" s="54" t="s">
+        <v>810</v>
+      </c>
+      <c r="I68" s="54" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B69" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C69" t="s">
+        <v>724</v>
+      </c>
+      <c r="D69" t="s">
+        <v>790</v>
+      </c>
+      <c r="E69" t="s">
+        <v>731</v>
+      </c>
+      <c r="F69" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G69" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H69" s="54" t="s">
+        <v>810</v>
+      </c>
+      <c r="I69" s="54" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B70" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C70" t="s">
+        <v>779</v>
+      </c>
+      <c r="D70" t="s">
+        <v>789</v>
+      </c>
+      <c r="E70" t="s">
+        <v>731</v>
+      </c>
+      <c r="F70" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G70" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H70" s="54" t="s">
+        <v>810</v>
+      </c>
+      <c r="I70" s="54" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B71" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C71" t="s">
+        <v>780</v>
+      </c>
+      <c r="D71" t="s">
+        <v>791</v>
+      </c>
+      <c r="E71" t="s">
+        <v>731</v>
+      </c>
+      <c r="F71" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G71" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H71" s="54" t="s">
+        <v>809</v>
+      </c>
+      <c r="I71" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B72" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C72" t="s">
+        <v>781</v>
+      </c>
+      <c r="D72" t="s">
+        <v>792</v>
+      </c>
+      <c r="E72" t="s">
+        <v>731</v>
+      </c>
+      <c r="F72" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G72" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H72" s="54" t="s">
+        <v>809</v>
+      </c>
+      <c r="I72" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B73" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C73" t="s">
+        <v>803</v>
+      </c>
+      <c r="D73" t="s">
+        <v>804</v>
+      </c>
+      <c r="E73" t="s">
+        <v>731</v>
+      </c>
+      <c r="F73" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G73" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H73" s="54" t="s">
+        <v>809</v>
+      </c>
+      <c r="I73" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B74" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C74" t="s">
+        <v>782</v>
+      </c>
+      <c r="D74" t="s">
+        <v>802</v>
+      </c>
+      <c r="E74" t="s">
+        <v>731</v>
+      </c>
+      <c r="F74" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G74" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H74" s="54" t="s">
+        <v>809</v>
+      </c>
+      <c r="I74" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="54" t="s">
+        <v>659</v>
+      </c>
+      <c r="B75" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C75" t="s">
+        <v>783</v>
+      </c>
+      <c r="D75" t="s">
+        <v>793</v>
+      </c>
+      <c r="E75" t="s">
+        <v>731</v>
+      </c>
+      <c r="F75" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G75" s="54" t="s">
+        <v>730</v>
+      </c>
+      <c r="H75" s="54" t="s">
+        <v>809</v>
+      </c>
+      <c r="I75" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B76" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C76" t="s">
+        <v>780</v>
+      </c>
+      <c r="D76" s="54" t="s">
+        <v>797</v>
+      </c>
+      <c r="E76" t="s">
+        <v>731</v>
+      </c>
+      <c r="F76" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G76" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H76" t="s">
+        <v>798</v>
+      </c>
+      <c r="I76" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B77" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C77" t="s">
+        <v>781</v>
+      </c>
+      <c r="D77" s="54" t="s">
+        <v>799</v>
+      </c>
+      <c r="E77" t="s">
+        <v>731</v>
+      </c>
+      <c r="F77" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G77" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H77" t="s">
+        <v>798</v>
+      </c>
+      <c r="I77" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B78" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C78" t="s">
+        <v>803</v>
+      </c>
+      <c r="D78" s="54" t="s">
+        <v>800</v>
+      </c>
+      <c r="E78" t="s">
+        <v>731</v>
+      </c>
+      <c r="F78" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G78" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H78" t="s">
+        <v>798</v>
+      </c>
+      <c r="I78" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B79" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C79" t="s">
+        <v>782</v>
+      </c>
+      <c r="D79" s="54" t="s">
+        <v>801</v>
+      </c>
+      <c r="E79" t="s">
+        <v>731</v>
+      </c>
+      <c r="F79" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G79" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H79" t="s">
+        <v>798</v>
+      </c>
+      <c r="I79" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="54" t="s">
+        <v>646</v>
+      </c>
+      <c r="B80" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="C80" t="s">
+        <v>783</v>
+      </c>
+      <c r="D80" s="54" t="s">
+        <v>805</v>
+      </c>
+      <c r="E80" t="s">
+        <v>731</v>
+      </c>
+      <c r="F80" s="54" t="s">
+        <v>647</v>
+      </c>
+      <c r="G80" s="54" t="s">
+        <v>798</v>
+      </c>
+      <c r="H80" t="s">
+        <v>798</v>
+      </c>
+      <c r="I80" t="s">
+        <v>813</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A34:A35 A62:A80 A2:A23">
       <formula1>"Input,Output,Calculated"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>"General,PD,LGD,CCF,ELBE,LGDD,SL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F80">
       <formula1>"Datetime,Categorical,Numeric"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="33ef62f9-2e07-484b-bd79-00aec90129fe" ContentTypeId="0x010100826318CDA76982469C2C3CD2CD5847410101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -16517,97 +17893,12 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="33ef62f9-2e07-484b-bd79-00aec90129fe" ContentTypeId="0x010100826318CDA76982469C2C3CD2CD5847410101" PreviousValue="false"/>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <jc981bd8ab5b47fd91abb7684c0f405b xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Brussels</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0086b60c-6752-48fa-8e91-a8805d8608ed</TermId>
-        </TermInfo>
-      </Terms>
-    </jc981bd8ab5b47fd91abb7684c0f405b>
-    <i14ea8bbd518495ea0e20ac1ad18c527 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Campaign Materials</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10e3cb14-f0bd-4a0a-bb1a-58c7e26fd5e4</TermId>
-        </TermInfo>
-      </Terms>
-    </i14ea8bbd518495ea0e20ac1ad18c527>
-    <b4187e12891e46deb4d240a4b28bdb90 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b4187e12891e46deb4d240a4b28bdb90>
-    <TaxCatchAll xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Value>13</Value>
-      <Value>12</Value>
-      <Value>11</Value>
-    </TaxCatchAll>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <e0e024ccac5240e69ae9c38a41bfa7a5 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </e0e024ccac5240e69ae9c38a41bfa7a5>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <Classification_x0020_Status xmlns="35818088-e62d-4edf-bbb6-409430aef268" xsi:nil="true"/>
-    <k8128b1c45734e36a24fce652bc7ffb7 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Quantitative Services</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8ac922a9-ccce-4035-83d6-3ab1113bed22</TermId>
-        </TermInfo>
-      </Terms>
-    </k8128b1c45734e36a24fce652bc7ffb7>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-    <_dlc_DocId xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">3KSVPJYEA2AR-1011915566-26</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
-      <Url>https://sites.ey.com/sites/QAS_BELGIUM/_layouts/15/DocIdRedir.aspx?ID=3KSVPJYEA2AR-1011915566-26</Url>
-      <Description>3KSVPJYEA2AR-1011915566-26</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
-      <UserInfo>
-        <DisplayName>Diego De Plaen</DisplayName>
-        <AccountId>56</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Antonio Millan Puebla</DisplayName>
-        <AccountId>31</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sander Vandevenne</DisplayName>
-        <AccountId>54</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="EY Collaboration Document" ma:contentTypeID="0x010100826318CDA76982469C2C3CD2CD58474101010039A9718220E30744AB05D9570037D8A1" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0a3d079c8d19385a693d7ea59f238e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="50c908b1-f277-4340-90a9-4611d0b0f078" xmlns:ns4="35818088-e62d-4edf-bbb6-409430aef268" xmlns:ns5="40c6704c-f77c-4b8a-96a1-a10a2e12c42b" xmlns:ns6="96860b88-8044-411d-9267-72f1d28f5ec3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0684eb5fe437c3d422fbfa93671a941" ns1:_="" ns2:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16952,7 +18243,105 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <jc981bd8ab5b47fd91abb7684c0f405b xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Brussels</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0086b60c-6752-48fa-8e91-a8805d8608ed</TermId>
+        </TermInfo>
+      </Terms>
+    </jc981bd8ab5b47fd91abb7684c0f405b>
+    <i14ea8bbd518495ea0e20ac1ad18c527 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Campaign Materials</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10e3cb14-f0bd-4a0a-bb1a-58c7e26fd5e4</TermId>
+        </TermInfo>
+      </Terms>
+    </i14ea8bbd518495ea0e20ac1ad18c527>
+    <b4187e12891e46deb4d240a4b28bdb90 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b4187e12891e46deb4d240a4b28bdb90>
+    <TaxCatchAll xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Value>13</Value>
+      <Value>12</Value>
+      <Value>11</Value>
+    </TaxCatchAll>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <e0e024ccac5240e69ae9c38a41bfa7a5 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e0e024ccac5240e69ae9c38a41bfa7a5>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <Classification_x0020_Status xmlns="35818088-e62d-4edf-bbb6-409430aef268" xsi:nil="true"/>
+    <k8128b1c45734e36a24fce652bc7ffb7 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Quantitative Services</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8ac922a9-ccce-4035-83d6-3ab1113bed22</TermId>
+        </TermInfo>
+      </Terms>
+    </k8128b1c45734e36a24fce652bc7ffb7>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+    <_dlc_DocId xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">3KSVPJYEA2AR-1011915566-26</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
+      <Url>https://sites.ey.com/sites/QAS_BELGIUM/_layouts/15/DocIdRedir.aspx?ID=3KSVPJYEA2AR-1011915566-26</Url>
+      <Description>3KSVPJYEA2AR-1011915566-26</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
+      <UserInfo>
+        <DisplayName>Diego De Plaen</DisplayName>
+        <AccountId>56</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Antonio Millan Puebla</DisplayName>
+        <AccountId>31</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sander Vandevenne</DisplayName>
+        <AccountId>54</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65E10CC5-2433-4DC9-9A6B-251C7485D767}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4AB6DE9-C584-4E87-8FF5-1A82C035629B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
@@ -16960,18 +18349,24 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65E10CC5-2433-4DC9-9A6B-251C7485D767}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2D0B982-DBCA-4EED-A652-6CD257CDA216}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D6130A-D52D-416E-88B9-F6885590E854}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="50c908b1-f277-4340-90a9-4611d0b0f078"/>
+    <ds:schemaRef ds:uri="35818088-e62d-4edf-bbb6-409430aef268"/>
+    <ds:schemaRef ds:uri="40c6704c-f77c-4b8a-96a1-a10a2e12c42b"/>
+    <ds:schemaRef ds:uri="96860b88-8044-411d-9267-72f1d28f5ec3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16997,23 +18392,9 @@
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2D0B982-DBCA-4EED-A652-6CD257CDA216}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D6130A-D52D-416E-88B9-F6885590E854}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="50c908b1-f277-4340-90a9-4611d0b0f078"/>
-    <ds:schemaRef ds:uri="35818088-e62d-4edf-bbb6-409430aef268"/>
-    <ds:schemaRef ds:uri="40c6704c-f77c-4b8a-96a1-a10a2e12c42b"/>
-    <ds:schemaRef ds:uri="96860b88-8044-411d-9267-72f1d28f5ec3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed the excel output range on backtesting output statistics
</commit_message>
<xml_diff>
--- a/IRB models/Data Model.xlsx
+++ b/IRB models/Data Model.xlsx
@@ -442,6 +442,113 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Sander Vandevenne</author>
+  </authors>
+  <commentList>
+    <comment ref="C97" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sander Vandevenne:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Expand computation of statistics
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C98" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sander Vandevenne:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Expand computation of statistics</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C99" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sander Vandevenne:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Expand computation of statistics</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C100" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sander Vandevenne:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Expand computation of statistics</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="951">
   <si>
@@ -3189,10 +3296,6 @@
     <t>backtesting</t>
   </si>
   <si>
-    <t xml:space="preserve">workbook: LEICode_LGD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
-sheet: 2.0      cell: V8 </t>
-  </si>
-  <si>
     <t>LGDD_realised</t>
   </si>
   <si>
@@ -3203,10 +3306,6 @@
   </si>
   <si>
     <t>LGDD_backtesting_perGrade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workbook: LEICode_LGDD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
-sheet: 2.0      cell: V8 </t>
   </si>
   <si>
     <t>LGDD_toExcel</t>
@@ -3364,27 +3463,36 @@
     <t>workbook: LEICode_CCF_ModelID_EndOfObservationPeriod_versionNumber.xlsx sheet: 5.2      cell: E40</t>
   </si>
   <si>
+    <t xml:space="preserve">workbook: LEICode_LGD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 2.0      cell: AD8:AF8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">workbook: LEICode_LGD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 2.0      cell: Range(.[AD10], .[AF10].End(xlDown)) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">workbook: LEICode_LGDD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 2.0      cell: H7:J7; O7:Q7; V7:X7; AC7:AE7; AJ7:AL7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">workbook: LEICode_LGDD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
+sheet: 2.0      cell: Range(.[H9], .[J9].End(xlDown)) ; Range(.[O9], .[Q9].End(xlDown)); Range(.[V9], .[X9].End(xlDown)); Range(.[AC9], .[AE9].End(xlDown)); Range(.[AJ9], .[AL9].End(xlDown)) 
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">workbook: LEICode_CCF_ModelID_EndOfObservationPeriod_versionNumber.xlsx
-sheet: 3.1      cell: U8 </t>
+sheet: 3.1      cell: T8:V8 </t>
   </si>
   <si>
     <t xml:space="preserve">workbook: LEICode_CCF_ModelID_EndOfObservationPeriod_versionNumber.xlsx
-sheet: 3.1      cell: Range(.[U10], .[U10].End(xlDown)) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">workbook: LEICode_LGDD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
-sheet: 2.0      cell: Range(.[V10], .[V10].End(xlDown)) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">workbook: LEICode_LGD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
-sheet: 2.0      cell: Range(.[V10], .[V10].End(xlDown)) </t>
+sheet: 3.1      cell: Range(.[T10], .[V10].End(xlDown)) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3594,6 +3702,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="41">
@@ -4473,6 +4594,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="37" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4521,7 +4643,6 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="88">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7809,74 +7930,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="95" t="s">
         <v>562</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="96"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="97"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="97"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="99"/>
+      <c r="A2" s="98"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="100"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="91" t="s">
         <v>563</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="92"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="93"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>564</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="101" t="s">
         <v>565</v>
       </c>
-      <c r="C5" s="101"/>
-      <c r="D5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="103"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>566</v>
       </c>
-      <c r="B6" s="100" t="s">
+      <c r="B6" s="101" t="s">
         <v>567</v>
       </c>
-      <c r="C6" s="101"/>
-      <c r="D6" s="102"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="103"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>568</v>
       </c>
-      <c r="B7" s="103" t="s">
+      <c r="B7" s="104" t="s">
         <v>569</v>
       </c>
-      <c r="C7" s="104"/>
-      <c r="D7" s="105"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="106"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
         <v>570</v>
       </c>
-      <c r="B8" s="103" t="s">
+      <c r="B8" s="104" t="s">
         <v>571</v>
       </c>
-      <c r="C8" s="104"/>
-      <c r="D8" s="105"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="106"/>
     </row>
     <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="90" t="s">
+      <c r="A10" s="91" t="s">
         <v>572</v>
       </c>
-      <c r="B10" s="91"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="92"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="93"/>
     </row>
     <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
@@ -7936,12 +8057,12 @@
     </row>
     <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="94" t="s">
         <v>585</v>
       </c>
-      <c r="B17" s="93"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="93"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="94"/>
     </row>
     <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -15769,12 +15890,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
+      <selection pane="bottomLeft" activeCell="A131" sqref="A131:XFD132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16468,10 +16589,10 @@
         <v>365</v>
       </c>
       <c r="C24" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D24" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="E24" t="s">
         <v>731</v>
@@ -16642,10 +16763,10 @@
         <v>365</v>
       </c>
       <c r="C30" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D30" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="E30" t="s">
         <v>731</v>
@@ -17724,7 +17845,7 @@
         <v>886</v>
       </c>
       <c r="D67" t="s">
-        <v>892</v>
+        <v>945</v>
       </c>
       <c r="E67" t="s">
         <v>731</v>
@@ -17753,7 +17874,7 @@
         <v>887</v>
       </c>
       <c r="D68" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
       <c r="E68" t="s">
         <v>731</v>
@@ -17982,7 +18103,7 @@
         <v>463</v>
       </c>
       <c r="C76" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="D76" t="s">
         <v>789</v>
@@ -18011,7 +18132,7 @@
         <v>463</v>
       </c>
       <c r="C77" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="D77" t="s">
         <v>788</v>
@@ -18098,7 +18219,7 @@
         <v>463</v>
       </c>
       <c r="C80" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D80" t="s">
         <v>802</v>
@@ -18185,7 +18306,7 @@
         <v>463</v>
       </c>
       <c r="C83" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="D83" t="s">
         <v>802</v>
@@ -18272,7 +18393,7 @@
         <v>463</v>
       </c>
       <c r="C86" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D86" t="s">
         <v>799</v>
@@ -18359,10 +18480,10 @@
         <v>463</v>
       </c>
       <c r="C89" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="D89" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="E89" t="s">
         <v>731</v>
@@ -18476,10 +18597,10 @@
         <v>463</v>
       </c>
       <c r="C93" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="D93" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="E93" t="s">
         <v>731</v>
@@ -18505,10 +18626,10 @@
         <v>463</v>
       </c>
       <c r="C94" t="s">
+        <v>930</v>
+      </c>
+      <c r="D94" t="s">
         <v>932</v>
-      </c>
-      <c r="D94" t="s">
-        <v>934</v>
       </c>
       <c r="E94" t="s">
         <v>731</v>
@@ -18537,7 +18658,7 @@
         <v>554</v>
       </c>
       <c r="D95" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="E95" t="s">
         <v>729</v>
@@ -18563,10 +18684,10 @@
         <v>554</v>
       </c>
       <c r="C96" s="89" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D96" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E96" t="s">
         <v>729</v>
@@ -18592,10 +18713,10 @@
         <v>554</v>
       </c>
       <c r="C97" s="89" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D97" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="E97" t="s">
         <v>731</v>
@@ -18606,10 +18727,10 @@
       <c r="G97" s="54" t="s">
         <v>730</v>
       </c>
-      <c r="H97" s="106" t="s">
-        <v>895</v>
-      </c>
-      <c r="I97" s="106" t="s">
+      <c r="H97" s="90" t="s">
+        <v>894</v>
+      </c>
+      <c r="I97" s="90" t="s">
         <v>891</v>
       </c>
     </row>
@@ -18621,10 +18742,10 @@
         <v>554</v>
       </c>
       <c r="C98" s="89" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D98" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E98" t="s">
         <v>731</v>
@@ -18635,10 +18756,10 @@
       <c r="G98" s="54" t="s">
         <v>730</v>
       </c>
-      <c r="H98" s="106" t="s">
-        <v>895</v>
-      </c>
-      <c r="I98" s="106" t="s">
+      <c r="H98" s="90" t="s">
+        <v>894</v>
+      </c>
+      <c r="I98" s="90" t="s">
         <v>890</v>
       </c>
     </row>
@@ -18650,10 +18771,10 @@
         <v>554</v>
       </c>
       <c r="C99" s="89" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D99" s="89" t="s">
-        <v>897</v>
+        <v>947</v>
       </c>
       <c r="E99" t="s">
         <v>731</v>
@@ -18664,11 +18785,11 @@
       <c r="G99" s="54" t="s">
         <v>797</v>
       </c>
-      <c r="H99" s="54" t="s">
+      <c r="H99" s="90" t="s">
         <v>797</v>
       </c>
-      <c r="I99" s="106" t="s">
-        <v>898</v>
+      <c r="I99" s="90" t="s">
+        <v>896</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
@@ -18679,10 +18800,10 @@
         <v>554</v>
       </c>
       <c r="C100" s="89" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D100" s="89" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="E100" t="s">
         <v>731</v>
@@ -18693,11 +18814,11 @@
       <c r="G100" s="54" t="s">
         <v>797</v>
       </c>
-      <c r="H100" s="54" t="s">
+      <c r="H100" s="90" t="s">
         <v>797</v>
       </c>
-      <c r="I100" s="106" t="s">
-        <v>898</v>
+      <c r="I100" s="90" t="s">
+        <v>896</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
@@ -18711,7 +18832,7 @@
         <v>499</v>
       </c>
       <c r="D101" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E101" t="s">
         <v>729</v>
@@ -18737,10 +18858,10 @@
         <v>499</v>
       </c>
       <c r="C102" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="D102" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="E102" t="s">
         <v>729</v>
@@ -18766,10 +18887,10 @@
         <v>499</v>
       </c>
       <c r="C103" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="D103" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="E103" t="s">
         <v>729</v>
@@ -18795,10 +18916,10 @@
         <v>499</v>
       </c>
       <c r="C104" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="D104" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="E104" t="s">
         <v>729</v>
@@ -18853,7 +18974,7 @@
         <v>499</v>
       </c>
       <c r="C106" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="D106" t="s">
         <v>786</v>
@@ -18882,7 +19003,7 @@
         <v>499</v>
       </c>
       <c r="C107" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="D107" t="s">
         <v>787</v>
@@ -18911,7 +19032,7 @@
         <v>499</v>
       </c>
       <c r="C108" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D108" t="s">
         <v>789</v>
@@ -18940,7 +19061,7 @@
         <v>499</v>
       </c>
       <c r="C109" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="D109" t="s">
         <v>788</v>
@@ -18969,7 +19090,7 @@
         <v>499</v>
       </c>
       <c r="C110" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="D110" t="s">
         <v>790</v>
@@ -18984,7 +19105,7 @@
         <v>730</v>
       </c>
       <c r="H110" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="I110" t="s">
         <v>721</v>
@@ -18998,7 +19119,7 @@
         <v>499</v>
       </c>
       <c r="C111" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="D111" t="s">
         <v>791</v>
@@ -19013,7 +19134,7 @@
         <v>730</v>
       </c>
       <c r="H111" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="I111" t="s">
         <v>721</v>
@@ -19027,10 +19148,10 @@
         <v>499</v>
       </c>
       <c r="C112" t="s">
+        <v>924</v>
+      </c>
+      <c r="D112" t="s">
         <v>926</v>
-      </c>
-      <c r="D112" t="s">
-        <v>928</v>
       </c>
       <c r="E112" t="s">
         <v>731</v>
@@ -19042,7 +19163,7 @@
         <v>730</v>
       </c>
       <c r="H112" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="I112" t="s">
         <v>721</v>
@@ -19056,7 +19177,7 @@
         <v>499</v>
       </c>
       <c r="C113" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="D113" t="s">
         <v>801</v>
@@ -19071,7 +19192,7 @@
         <v>730</v>
       </c>
       <c r="H113" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="I113" t="s">
         <v>721</v>
@@ -19085,7 +19206,7 @@
         <v>499</v>
       </c>
       <c r="C114" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="D114" t="s">
         <v>792</v>
@@ -19100,7 +19221,7 @@
         <v>730</v>
       </c>
       <c r="H114" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="I114" t="s">
         <v>721</v>
@@ -19114,7 +19235,7 @@
         <v>499</v>
       </c>
       <c r="C115" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D115" t="s">
         <v>802</v>
@@ -19129,7 +19250,7 @@
         <v>730</v>
       </c>
       <c r="H115" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="I115" t="s">
         <v>721</v>
@@ -19143,10 +19264,10 @@
         <v>499</v>
       </c>
       <c r="C116" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="D116" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="E116" t="s">
         <v>731</v>
@@ -19161,7 +19282,7 @@
         <v>797</v>
       </c>
       <c r="I116" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
@@ -19172,10 +19293,10 @@
         <v>499</v>
       </c>
       <c r="C117" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="D117" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="E117" t="s">
         <v>731</v>
@@ -19190,7 +19311,7 @@
         <v>797</v>
       </c>
       <c r="I117" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
@@ -19201,10 +19322,10 @@
         <v>499</v>
       </c>
       <c r="C118" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="D118" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="E118" t="s">
         <v>731</v>
@@ -19219,7 +19340,7 @@
         <v>797</v>
       </c>
       <c r="I118" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
@@ -19230,10 +19351,10 @@
         <v>499</v>
       </c>
       <c r="C119" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="D119" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="E119" t="s">
         <v>731</v>
@@ -19248,7 +19369,7 @@
         <v>797</v>
       </c>
       <c r="I119" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
@@ -19259,10 +19380,10 @@
         <v>499</v>
       </c>
       <c r="C120" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="D120" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="E120" t="s">
         <v>731</v>
@@ -19277,7 +19398,7 @@
         <v>797</v>
       </c>
       <c r="I120" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
@@ -19288,10 +19409,10 @@
         <v>499</v>
       </c>
       <c r="C121" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D121" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="E121" t="s">
         <v>731</v>
@@ -19306,7 +19427,7 @@
         <v>797</v>
       </c>
       <c r="I121" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
@@ -19320,7 +19441,7 @@
         <v>499</v>
       </c>
       <c r="D122" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E122" t="s">
         <v>729</v>
@@ -19346,10 +19467,10 @@
         <v>499</v>
       </c>
       <c r="C123" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="D123" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="E123" t="s">
         <v>729</v>
@@ -19405,10 +19526,10 @@
         <v>499</v>
       </c>
       <c r="C125" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="D125" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="E125" t="s">
         <v>731</v>
@@ -19420,7 +19541,7 @@
         <v>730</v>
       </c>
       <c r="H125" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="I125" t="s">
         <v>721</v>
@@ -19434,10 +19555,10 @@
         <v>499</v>
       </c>
       <c r="C126" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="D126" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="E126" t="s">
         <v>731</v>
@@ -19452,7 +19573,7 @@
         <v>797</v>
       </c>
       <c r="I126" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
@@ -19466,7 +19587,7 @@
         <v>499</v>
       </c>
       <c r="D127" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E127" t="s">
         <v>729</v>
@@ -19492,10 +19613,10 @@
         <v>499</v>
       </c>
       <c r="C128" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="D128" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="E128" t="s">
         <v>729</v>
@@ -19521,10 +19642,10 @@
         <v>499</v>
       </c>
       <c r="C129" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="D129" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="E129" t="s">
         <v>731</v>
@@ -19536,7 +19657,7 @@
         <v>730</v>
       </c>
       <c r="H129" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="I129" t="s">
         <v>891</v>
@@ -19550,10 +19671,10 @@
         <v>499</v>
       </c>
       <c r="C130" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="D130" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="E130" t="s">
         <v>731</v>
@@ -19565,7 +19686,7 @@
         <v>730</v>
       </c>
       <c r="H130" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="I130" t="s">
         <v>890</v>
@@ -19579,10 +19700,10 @@
         <v>499</v>
       </c>
       <c r="C131" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="D131" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E131" t="s">
         <v>731</v>
@@ -19597,7 +19718,7 @@
         <v>797</v>
       </c>
       <c r="I131" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
@@ -19608,10 +19729,10 @@
         <v>499</v>
       </c>
       <c r="C132" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="D132" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="E132" t="s">
         <v>731</v>
@@ -19626,7 +19747,7 @@
         <v>797</v>
       </c>
       <c r="I132" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
   </sheetData>
@@ -19644,150 +19765,11 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <jc981bd8ab5b47fd91abb7684c0f405b xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Brussels</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0086b60c-6752-48fa-8e91-a8805d8608ed</TermId>
-        </TermInfo>
-      </Terms>
-    </jc981bd8ab5b47fd91abb7684c0f405b>
-    <i14ea8bbd518495ea0e20ac1ad18c527 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Campaign Materials</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10e3cb14-f0bd-4a0a-bb1a-58c7e26fd5e4</TermId>
-        </TermInfo>
-      </Terms>
-    </i14ea8bbd518495ea0e20ac1ad18c527>
-    <b4187e12891e46deb4d240a4b28bdb90 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b4187e12891e46deb4d240a4b28bdb90>
-    <TaxCatchAll xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Value>13</Value>
-      <Value>12</Value>
-      <Value>11</Value>
-    </TaxCatchAll>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <e0e024ccac5240e69ae9c38a41bfa7a5 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </e0e024ccac5240e69ae9c38a41bfa7a5>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <Classification_x0020_Status xmlns="35818088-e62d-4edf-bbb6-409430aef268" xsi:nil="true"/>
-    <k8128b1c45734e36a24fce652bc7ffb7 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Quantitative Services</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8ac922a9-ccce-4035-83d6-3ab1113bed22</TermId>
-        </TermInfo>
-      </Terms>
-    </k8128b1c45734e36a24fce652bc7ffb7>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-    <_dlc_DocId xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">3KSVPJYEA2AR-1011915566-26</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
-      <Url>https://sites.ey.com/sites/QAS_BELGIUM/_layouts/15/DocIdRedir.aspx?ID=3KSVPJYEA2AR-1011915566-26</Url>
-      <Description>3KSVPJYEA2AR-1011915566-26</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
-      <UserInfo>
-        <DisplayName>Diego De Plaen</DisplayName>
-        <AccountId>56</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Antonio Millan Puebla</DisplayName>
-        <AccountId>31</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sander Vandevenne</DisplayName>
-        <AccountId>54</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="EY Collaboration Document" ma:contentTypeID="0x010100826318CDA76982469C2C3CD2CD58474101010039A9718220E30744AB05D9570037D8A1" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0a3d079c8d19385a693d7ea59f238e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="50c908b1-f277-4340-90a9-4611d0b0f078" xmlns:ns4="35818088-e62d-4edf-bbb6-409430aef268" xmlns:ns5="40c6704c-f77c-4b8a-96a1-a10a2e12c42b" xmlns:ns6="96860b88-8044-411d-9267-72f1d28f5ec3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0684eb5fe437c3d422fbfa93671a941" ns1:_="" ns2:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -20132,48 +20114,152 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <jc981bd8ab5b47fd91abb7684c0f405b xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Brussels</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0086b60c-6752-48fa-8e91-a8805d8608ed</TermId>
+        </TermInfo>
+      </Terms>
+    </jc981bd8ab5b47fd91abb7684c0f405b>
+    <i14ea8bbd518495ea0e20ac1ad18c527 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Campaign Materials</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10e3cb14-f0bd-4a0a-bb1a-58c7e26fd5e4</TermId>
+        </TermInfo>
+      </Terms>
+    </i14ea8bbd518495ea0e20ac1ad18c527>
+    <b4187e12891e46deb4d240a4b28bdb90 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b4187e12891e46deb4d240a4b28bdb90>
+    <TaxCatchAll xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Value>13</Value>
+      <Value>12</Value>
+      <Value>11</Value>
+    </TaxCatchAll>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <e0e024ccac5240e69ae9c38a41bfa7a5 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e0e024ccac5240e69ae9c38a41bfa7a5>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <Classification_x0020_Status xmlns="35818088-e62d-4edf-bbb6-409430aef268" xsi:nil="true"/>
+    <k8128b1c45734e36a24fce652bc7ffb7 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Quantitative Services</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8ac922a9-ccce-4035-83d6-3ab1113bed22</TermId>
+        </TermInfo>
+      </Terms>
+    </k8128b1c45734e36a24fce652bc7ffb7>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+    <_dlc_DocId xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">3KSVPJYEA2AR-1011915566-26</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
+      <Url>https://sites.ey.com/sites/QAS_BELGIUM/_layouts/15/DocIdRedir.aspx?ID=3KSVPJYEA2AR-1011915566-26</Url>
+      <Description>3KSVPJYEA2AR-1011915566-26</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
+      <UserInfo>
+        <DisplayName>Diego De Plaen</DisplayName>
+        <AccountId>56</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Antonio Millan Puebla</DisplayName>
+        <AccountId>31</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sander Vandevenne</DisplayName>
+        <AccountId>54</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="33ef62f9-2e07-484b-bd79-00aec90129fe" ContentTypeId="0x010100826318CDA76982469C2C3CD2CD5847410101" PreviousValue="false"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65E10CC5-2433-4DC9-9A6B-251C7485D767}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D6130A-D52D-416E-88B9-F6885590E854}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A2966CE-FBFB-42D6-8AF5-4361359F35A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="50c908b1-f277-4340-90a9-4611d0b0f078"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="35818088-e62d-4edf-bbb6-409430aef268"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="96860b88-8044-411d-9267-72f1d28f5ec3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="40c6704c-f77c-4b8a-96a1-a10a2e12c42b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2D0B982-DBCA-4EED-A652-6CD257CDA216}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20195,6 +20281,42 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A2966CE-FBFB-42D6-8AF5-4361359F35A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="50c908b1-f277-4340-90a9-4611d0b0f078"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="35818088-e62d-4edf-bbb6-409430aef268"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="96860b88-8044-411d-9267-72f1d28f5ec3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="40c6704c-f77c-4b8a-96a1-a10a2e12c42b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D6130A-D52D-416E-88B9-F6885590E854}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65E10CC5-2433-4DC9-9A6B-251C7485D767}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4AB6DE9-C584-4E87-8FF5-1A82C035629B}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Removed marking of HI exp calculation (since it has been implemented)
</commit_message>
<xml_diff>
--- a/IRB models/Data Model.xlsx
+++ b/IRB models/Data Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bebxadvboey\Documents\Python\GitHub\ML4Credit\IRB models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0EC9164C-3B16-40D6-B8E5-E9A533FFB988}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{40C4E77E-7514-4059-9C4B-DE8DEAE3C9B3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" state="hidden" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -9253,7 +9253,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -10755,9 +10755,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12384,7 +12384,7 @@
       <c r="B56" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="38" t="s">
         <v>415</v>
       </c>
       <c r="D56" t="s">
@@ -12413,7 +12413,7 @@
       <c r="B57" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="38" t="s">
         <v>524</v>
       </c>
       <c r="D57" t="s">
@@ -12442,7 +12442,7 @@
       <c r="B58" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="C58" s="39" t="s">
+      <c r="C58" s="38" t="s">
         <v>525</v>
       </c>
       <c r="D58" t="s">
@@ -12471,7 +12471,7 @@
       <c r="B59" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="38" t="s">
         <v>414</v>
       </c>
       <c r="D59" t="s">
@@ -12500,7 +12500,7 @@
       <c r="B60" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="38" t="s">
         <v>415</v>
       </c>
       <c r="D60" t="s">
@@ -12529,7 +12529,7 @@
       <c r="B61" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="38" t="s">
         <v>524</v>
       </c>
       <c r="D61" t="s">
@@ -12558,7 +12558,7 @@
       <c r="B62" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="C62" s="39" t="s">
+      <c r="C62" s="38" t="s">
         <v>525</v>
       </c>
       <c r="D62" t="s">
@@ -12587,7 +12587,7 @@
       <c r="B63" s="35" t="s">
         <v>361</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="38" t="s">
         <v>361</v>
       </c>
       <c r="D63" t="s">
@@ -14939,6 +14939,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="33ef62f9-2e07-484b-bd79-00aec90129fe" ContentTypeId="0x010100826318CDA76982469C2C3CD2CD5847410101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="EY Collaboration Document" ma:contentTypeID="0x010100826318CDA76982469C2C3CD2CD58474101010039A9718220E30744AB05D9570037D8A1" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0a3d079c8d19385a693d7ea59f238e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="50c908b1-f277-4340-90a9-4611d0b0f078" xmlns:ns4="35818088-e62d-4edf-bbb6-409430aef268" xmlns:ns5="40c6704c-f77c-4b8a-96a1-a10a2e12c42b" xmlns:ns6="96860b88-8044-411d-9267-72f1d28f5ec3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0684eb5fe437c3d422fbfa93671a941" ns1:_="" ns2:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15283,71 +15288,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="33ef62f9-2e07-484b-bd79-00aec90129fe" ContentTypeId="0x010100826318CDA76982469C2C3CD2CD5847410101" PreviousValue="false"/>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -15428,7 +15369,74 @@
 </p:properties>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4AB6DE9-C584-4E87-8FF5-1A82C035629B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2D0B982-DBCA-4EED-A652-6CD257CDA216}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15450,31 +15458,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4AB6DE9-C584-4E87-8FF5-1A82C035629B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65E10CC5-2433-4DC9-9A6B-251C7485D767}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D6130A-D52D-416E-88B9-F6885590E854}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A2966CE-FBFB-42D6-8AF5-4361359F35A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -15492,4 +15476,20 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D6130A-D52D-416E-88B9-F6885590E854}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65E10CC5-2433-4DC9-9A6B-251C7485D767}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Small update in nomenclatur for qualitative PD technical variables
</commit_message>
<xml_diff>
--- a/IRB models/Data Model.xlsx
+++ b/IRB models/Data Model.xlsx
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="631">
   <si>
     <t>LoanStatNew</t>
   </si>
@@ -2009,15 +2009,6 @@
     <t>PD_N</t>
   </si>
   <si>
-    <t>M_ex_ORFS</t>
-  </si>
-  <si>
-    <t>M_ex_TR</t>
-  </si>
-  <si>
-    <t>M_ex_EPD</t>
-  </si>
-  <si>
     <t>workbook: LEICode_PD_ModelID_EndOfObservationPeriod_versionNumber.xlsx
 sheet: 2.0      cell: E6</t>
   </si>
@@ -2096,6 +2087,12 @@
   </si>
   <si>
     <t>Section 2.3(f)</t>
+  </si>
+  <si>
+    <t>PD_M_ex_TR</t>
+  </si>
+  <si>
+    <t>PD_M_ex_EPD</t>
   </si>
 </sst>
 </file>
@@ -3061,6 +3058,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="13" fillId="37" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3109,8 +3108,6 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
   </cellXfs>
   <cellStyles count="88">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -10858,8 +10855,8 @@
   <dimension ref="A1:I154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10994,502 +10991,502 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="41" t="s">
         <v>410</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="42" t="s">
         <v>602</v>
       </c>
-      <c r="D5" s="58" t="s">
-        <v>631</v>
-      </c>
-      <c r="E5" s="58" t="s">
+      <c r="D5" s="42" t="s">
+        <v>628</v>
+      </c>
+      <c r="E5" s="42" t="s">
         <v>419</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="42" t="s">
         <v>412</v>
       </c>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="41" t="s">
         <v>410</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="42" t="s">
+        <v>613</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>623</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>419</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="41" t="s">
+        <v>413</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>614</v>
+      </c>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42" t="s">
+        <v>419</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="41" t="s">
+        <v>413</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>615</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42" t="s">
+        <v>419</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="41" t="s">
+        <v>410</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>629</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>624</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>419</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="41" t="s">
+        <v>413</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C10" s="42" t="s">
         <v>616</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D10" s="42"/>
+      <c r="E10" s="42" t="s">
+        <v>419</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="41" t="s">
+        <v>413</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>617</v>
+      </c>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42" t="s">
+        <v>419</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="41" t="s">
+        <v>410</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>630</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>622</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>419</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="41" t="s">
+        <v>410</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>605</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>625</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>419</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="41" t="s">
+        <v>410</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>603</v>
+      </c>
+      <c r="D14" s="42" t="s">
         <v>626</v>
       </c>
-      <c r="E6" s="58" t="s">
+      <c r="E14" s="42" t="s">
         <v>419</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F14" s="42" t="s">
         <v>412</v>
       </c>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="57" t="s">
-        <v>413</v>
-      </c>
-      <c r="B7" s="57" t="s">
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="41" t="s">
+        <v>410</v>
+      </c>
+      <c r="B15" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C15" s="42" t="s">
+        <v>604</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>627</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>419</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>602</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>606</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="F16" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>613</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>607</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>614</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>618</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="F18" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>615</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>619</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>629</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>608</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="F20" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>616</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>620</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>412</v>
+      </c>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="C22" s="42" t="s">
         <v>617</v>
       </c>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58" t="s">
-        <v>419</v>
-      </c>
-      <c r="F7" s="58" t="s">
+      <c r="D22" s="42" t="s">
+        <v>621</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="F22" s="42" t="s">
         <v>412</v>
       </c>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="57" t="s">
-        <v>413</v>
-      </c>
-      <c r="B8" s="57" t="s">
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="B23" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="C8" s="58" t="s">
-        <v>618</v>
-      </c>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58" t="s">
-        <v>419</v>
-      </c>
-      <c r="F8" s="58" t="s">
+      <c r="C23" s="42" t="s">
+        <v>630</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>609</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="F23" s="42" t="s">
         <v>412</v>
       </c>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="57" t="s">
-        <v>410</v>
-      </c>
-      <c r="B9" s="57" t="s">
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="B24" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="C9" s="58" t="s">
-        <v>607</v>
-      </c>
-      <c r="D9" s="58" t="s">
-        <v>627</v>
-      </c>
-      <c r="E9" s="58" t="s">
-        <v>419</v>
-      </c>
-      <c r="F9" s="58" t="s">
+      <c r="C24" s="42" t="s">
+        <v>605</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>610</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="F24" s="42" t="s">
         <v>412</v>
       </c>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="57" t="s">
-        <v>413</v>
-      </c>
-      <c r="B10" s="57" t="s">
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="B25" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="C10" s="58" t="s">
-        <v>619</v>
-      </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58" t="s">
-        <v>419</v>
-      </c>
-      <c r="F10" s="58" t="s">
+      <c r="C25" s="42" t="s">
+        <v>603</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>612</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="F25" s="42" t="s">
         <v>412</v>
       </c>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="57" t="s">
-        <v>413</v>
-      </c>
-      <c r="B11" s="57" t="s">
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="B26" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="C11" s="58" t="s">
-        <v>620</v>
-      </c>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58" t="s">
-        <v>419</v>
-      </c>
-      <c r="F11" s="58" t="s">
+      <c r="C26" s="42" t="s">
+        <v>604</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>611</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>421</v>
+      </c>
+      <c r="F26" s="42" t="s">
         <v>412</v>
       </c>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="57" t="s">
-        <v>410</v>
-      </c>
-      <c r="B12" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C12" s="58" t="s">
-        <v>608</v>
-      </c>
-      <c r="D12" s="58" t="s">
-        <v>625</v>
-      </c>
-      <c r="E12" s="58" t="s">
-        <v>419</v>
-      </c>
-      <c r="F12" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="57" t="s">
-        <v>410</v>
-      </c>
-      <c r="B13" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C13" s="58" t="s">
-        <v>605</v>
-      </c>
-      <c r="D13" s="58" t="s">
-        <v>628</v>
-      </c>
-      <c r="E13" s="58" t="s">
-        <v>419</v>
-      </c>
-      <c r="F13" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="57" t="s">
-        <v>410</v>
-      </c>
-      <c r="B14" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C14" s="58" t="s">
-        <v>603</v>
-      </c>
-      <c r="D14" s="58" t="s">
-        <v>629</v>
-      </c>
-      <c r="E14" s="58" t="s">
-        <v>419</v>
-      </c>
-      <c r="F14" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="57" t="s">
-        <v>410</v>
-      </c>
-      <c r="B15" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C15" s="58" t="s">
-        <v>604</v>
-      </c>
-      <c r="D15" s="58" t="s">
-        <v>630</v>
-      </c>
-      <c r="E15" s="58" t="s">
-        <v>419</v>
-      </c>
-      <c r="F15" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="B16" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C16" s="58" t="s">
-        <v>602</v>
-      </c>
-      <c r="D16" s="58" t="s">
-        <v>609</v>
-      </c>
-      <c r="E16" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="F16" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="B17" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C17" s="58" t="s">
-        <v>606</v>
-      </c>
-      <c r="D17" s="58" t="s">
-        <v>610</v>
-      </c>
-      <c r="E17" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="F17" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="B18" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C18" s="58" t="s">
-        <v>617</v>
-      </c>
-      <c r="D18" s="58" t="s">
-        <v>621</v>
-      </c>
-      <c r="E18" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="F18" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="B19" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C19" s="58" t="s">
-        <v>618</v>
-      </c>
-      <c r="D19" s="58" t="s">
-        <v>622</v>
-      </c>
-      <c r="E19" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="F19" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="B20" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C20" s="58" t="s">
-        <v>607</v>
-      </c>
-      <c r="D20" s="58" t="s">
-        <v>611</v>
-      </c>
-      <c r="E20" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="F20" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="B21" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C21" s="58" t="s">
-        <v>619</v>
-      </c>
-      <c r="D21" s="58" t="s">
-        <v>623</v>
-      </c>
-      <c r="E21" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="F21" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="B22" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C22" s="58" t="s">
-        <v>620</v>
-      </c>
-      <c r="D22" s="58" t="s">
-        <v>624</v>
-      </c>
-      <c r="E22" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="F22" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="B23" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C23" s="58" t="s">
-        <v>608</v>
-      </c>
-      <c r="D23" s="58" t="s">
-        <v>612</v>
-      </c>
-      <c r="E23" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="F23" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="B24" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C24" s="58" t="s">
-        <v>605</v>
-      </c>
-      <c r="D24" s="58" t="s">
-        <v>613</v>
-      </c>
-      <c r="E24" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="F24" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="B25" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C25" s="58" t="s">
-        <v>603</v>
-      </c>
-      <c r="D25" s="58" t="s">
-        <v>615</v>
-      </c>
-      <c r="E25" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="F25" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="57" t="s">
-        <v>411</v>
-      </c>
-      <c r="B26" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C26" s="58" t="s">
-        <v>604</v>
-      </c>
-      <c r="D26" s="58" t="s">
-        <v>614</v>
-      </c>
-      <c r="E26" s="58" t="s">
-        <v>421</v>
-      </c>
-      <c r="F26" s="58" t="s">
-        <v>412</v>
-      </c>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="35" t="s">
@@ -15265,74 +15262,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>364</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="52"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="43" t="s">
         <v>365</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="43"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="45"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="53" t="s">
         <v>367</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>368</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="53" t="s">
         <v>369</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="53"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="55"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>370</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="56" t="s">
         <v>371</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="56"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>372</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="56" t="s">
         <v>373</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="56"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="58"/>
     </row>
     <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="43" t="s">
         <v>374</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="43"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="45"/>
     </row>
     <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
@@ -15392,12 +15389,12 @@
     </row>
     <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="46" t="s">
         <v>387</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
     </row>
     <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -15539,11 +15536,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="33ef62f9-2e07-484b-bd79-00aec90129fe" ContentTypeId="0x010100826318CDA76982469C2C3CD2CD5847410101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -15593,97 +15585,12 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="33ef62f9-2e07-484b-bd79-00aec90129fe" ContentTypeId="0x010100826318CDA76982469C2C3CD2CD5847410101" PreviousValue="false"/>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <jc981bd8ab5b47fd91abb7684c0f405b xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Brussels</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0086b60c-6752-48fa-8e91-a8805d8608ed</TermId>
-        </TermInfo>
-      </Terms>
-    </jc981bd8ab5b47fd91abb7684c0f405b>
-    <i14ea8bbd518495ea0e20ac1ad18c527 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Campaign Materials</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10e3cb14-f0bd-4a0a-bb1a-58c7e26fd5e4</TermId>
-        </TermInfo>
-      </Terms>
-    </i14ea8bbd518495ea0e20ac1ad18c527>
-    <b4187e12891e46deb4d240a4b28bdb90 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b4187e12891e46deb4d240a4b28bdb90>
-    <TaxCatchAll xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Value>13</Value>
-      <Value>12</Value>
-      <Value>11</Value>
-    </TaxCatchAll>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <e0e024ccac5240e69ae9c38a41bfa7a5 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </e0e024ccac5240e69ae9c38a41bfa7a5>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <Classification_x0020_Status xmlns="35818088-e62d-4edf-bbb6-409430aef268" xsi:nil="true"/>
-    <k8128b1c45734e36a24fce652bc7ffb7 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Quantitative Services</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8ac922a9-ccce-4035-83d6-3ab1113bed22</TermId>
-        </TermInfo>
-      </Terms>
-    </k8128b1c45734e36a24fce652bc7ffb7>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-    <_dlc_DocId xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">3KSVPJYEA2AR-1011915566-26</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
-      <Url>https://sites.ey.com/sites/QAS_BELGIUM/_layouts/15/DocIdRedir.aspx?ID=3KSVPJYEA2AR-1011915566-26</Url>
-      <Description>3KSVPJYEA2AR-1011915566-26</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
-      <UserInfo>
-        <DisplayName>Diego De Plaen</DisplayName>
-        <AccountId>56</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Antonio Millan Puebla</DisplayName>
-        <AccountId>31</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Sander Vandevenne</DisplayName>
-        <AccountId>54</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="EY Collaboration Document" ma:contentTypeID="0x010100826318CDA76982469C2C3CD2CD58474101010039A9718220E30744AB05D9570037D8A1" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0a3d079c8d19385a693d7ea59f238e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="50c908b1-f277-4340-90a9-4611d0b0f078" xmlns:ns4="35818088-e62d-4edf-bbb6-409430aef268" xmlns:ns5="40c6704c-f77c-4b8a-96a1-a10a2e12c42b" xmlns:ns6="96860b88-8044-411d-9267-72f1d28f5ec3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0684eb5fe437c3d422fbfa93671a941" ns1:_="" ns2:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16028,7 +15935,105 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <jc981bd8ab5b47fd91abb7684c0f405b xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Brussels</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">0086b60c-6752-48fa-8e91-a8805d8608ed</TermId>
+        </TermInfo>
+      </Terms>
+    </jc981bd8ab5b47fd91abb7684c0f405b>
+    <i14ea8bbd518495ea0e20ac1ad18c527 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Internal Campaign Materials</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10e3cb14-f0bd-4a0a-bb1a-58c7e26fd5e4</TermId>
+        </TermInfo>
+      </Terms>
+    </i14ea8bbd518495ea0e20ac1ad18c527>
+    <b4187e12891e46deb4d240a4b28bdb90 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b4187e12891e46deb4d240a4b28bdb90>
+    <TaxCatchAll xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Value>13</Value>
+      <Value>12</Value>
+      <Value>11</Value>
+    </TaxCatchAll>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <e0e024ccac5240e69ae9c38a41bfa7a5 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e0e024ccac5240e69ae9c38a41bfa7a5>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <Classification_x0020_Status xmlns="35818088-e62d-4edf-bbb6-409430aef268" xsi:nil="true"/>
+    <k8128b1c45734e36a24fce652bc7ffb7 xmlns="50c908b1-f277-4340-90a9-4611d0b0f078">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Quantitative Services</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8ac922a9-ccce-4035-83d6-3ab1113bed22</TermId>
+        </TermInfo>
+      </Terms>
+    </k8128b1c45734e36a24fce652bc7ffb7>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+    <_dlc_DocId xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">3KSVPJYEA2AR-1011915566-26</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
+      <Url>https://sites.ey.com/sites/QAS_BELGIUM/_layouts/15/DocIdRedir.aspx?ID=3KSVPJYEA2AR-1011915566-26</Url>
+      <Description>3KSVPJYEA2AR-1011915566-26</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="40c6704c-f77c-4b8a-96a1-a10a2e12c42b">
+      <UserInfo>
+        <DisplayName>Diego De Plaen</DisplayName>
+        <AccountId>56</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Antonio Millan Puebla</DisplayName>
+        <AccountId>31</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Sander Vandevenne</DisplayName>
+        <AccountId>54</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65E10CC5-2433-4DC9-9A6B-251C7485D767}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4AB6DE9-C584-4E87-8FF5-1A82C035629B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
@@ -16036,18 +16041,24 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65E10CC5-2433-4DC9-9A6B-251C7485D767}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2D0B982-DBCA-4EED-A652-6CD257CDA216}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D6130A-D52D-416E-88B9-F6885590E854}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="50c908b1-f277-4340-90a9-4611d0b0f078"/>
+    <ds:schemaRef ds:uri="35818088-e62d-4edf-bbb6-409430aef268"/>
+    <ds:schemaRef ds:uri="40c6704c-f77c-4b8a-96a1-a10a2e12c42b"/>
+    <ds:schemaRef ds:uri="96860b88-8044-411d-9267-72f1d28f5ec3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16073,23 +16084,9 @@
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2D0B982-DBCA-4EED-A652-6CD257CDA216}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D6130A-D52D-416E-88B9-F6885590E854}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="50c908b1-f277-4340-90a9-4611d0b0f078"/>
-    <ds:schemaRef ds:uri="35818088-e62d-4edf-bbb6-409430aef268"/>
-    <ds:schemaRef ds:uri="40c6704c-f77c-4b8a-96a1-a10a2e12c42b"/>
-    <ds:schemaRef ds:uri="96860b88-8044-411d-9267-72f1d28f5ec3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>